<commit_message>
meal updated 1 tarikh
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="11">
     <font>
       <sz val="11"/>
@@ -551,18 +551,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -678,19 +678,39 @@
       <c r="J4" s="6">
         <v>44470</v>
       </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
+      <c r="K4" s="4">
+        <v>5</v>
+      </c>
+      <c r="L4" s="4">
+        <v>2</v>
+      </c>
+      <c r="M4" s="4">
+        <v>2</v>
+      </c>
+      <c r="N4" s="4">
+        <v>2</v>
+      </c>
+      <c r="O4" s="4">
+        <v>1</v>
+      </c>
+      <c r="P4" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>0</v>
+      </c>
+      <c r="R4" s="4">
+        <v>2</v>
+      </c>
+      <c r="S4" s="4">
+        <v>1</v>
+      </c>
+      <c r="T4" s="4">
+        <v>2</v>
+      </c>
       <c r="U4" s="8">
         <f>SUM(K4:T4)</f>
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -703,7 +723,9 @@
       <c r="E5" s="6">
         <v>44471</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7">
+        <v>303</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -1113,7 +1135,7 @@
       </c>
       <c r="B18" s="11">
         <f>B13-F35</f>
-        <v>0</v>
+        <v>-303</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1640,7 +1662,7 @@
       </c>
       <c r="F35" s="12">
         <f>SUM(F4:F34)</f>
-        <v>2000</v>
+        <v>2303</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -1650,27 +1672,27 @@
       </c>
       <c r="K35" s="14">
         <f>SUM(K4:K34)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L35" s="14">
         <f>SUM(L4:L34)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M35" s="14">
         <f t="shared" ref="M35:T35" si="2">SUM(M4:M34)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N35" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O35" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q35" s="14">
         <f t="shared" si="2"/>
@@ -1678,19 +1700,19 @@
       </c>
       <c r="R35" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S35" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T35" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U35" s="15">
         <f>SUM(U4:U34)</f>
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:21">
@@ -1706,45 +1728,45 @@
       <c r="J36" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K36" s="4" t="e">
+      <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L36" s="4" t="e">
+        <v>606.0526315789474</v>
+      </c>
+      <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M36" s="4" t="e">
+        <v>242.42105263157896</v>
+      </c>
+      <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N36" s="4" t="e">
+        <v>242.42105263157896</v>
+      </c>
+      <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O36" s="4" t="e">
+        <v>242.42105263157896</v>
+      </c>
+      <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P36" s="4" t="e">
+        <v>121.21052631578948</v>
+      </c>
+      <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q36" s="4" t="e">
+        <v>242.42105263157896</v>
+      </c>
+      <c r="Q36" s="4">
         <f>Q35*B38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R36" s="4" t="e">
+        <v>0</v>
+      </c>
+      <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S36" s="4" t="e">
+        <v>242.42105263157896</v>
+      </c>
+      <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T36" s="4" t="e">
+        <v>121.21052631578948</v>
+      </c>
+      <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>#DIV/0!</v>
+        <v>242.42105263157896</v>
       </c>
       <c r="U36" s="8"/>
     </row>
@@ -1759,45 +1781,45 @@
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
-      <c r="K37" s="17" t="e">
+      <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L37" s="17" t="e">
+        <v>1393.9473684210525</v>
+      </c>
+      <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M37" s="21" t="e">
+        <v>-242.42105263157896</v>
+      </c>
+      <c r="M37" s="21">
         <f>B9-M36</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N37" s="17" t="e">
+        <v>-242.42105263157896</v>
+      </c>
+      <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O37" s="17" t="e">
+        <v>-242.42105263157896</v>
+      </c>
+      <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P37" s="17" t="e">
+        <v>-121.21052631578948</v>
+      </c>
+      <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q37" s="17" t="e">
+        <v>-242.42105263157896</v>
+      </c>
+      <c r="Q37" s="17">
         <f>B8-Q36</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R37" s="17" t="e">
+        <v>0</v>
+      </c>
+      <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S37" s="17" t="e">
+        <v>-242.42105263157896</v>
+      </c>
+      <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T37" s="17" t="e">
+        <v>-121.21052631578948</v>
+      </c>
+      <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>#DIV/0!</v>
+        <v>-242.42105263157896</v>
       </c>
       <c r="U37" s="8"/>
     </row>
@@ -1805,9 +1827,9 @@
       <c r="A38" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="18" t="e">
+      <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>#DIV/0!</v>
+        <v>121.21052631578948</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>

</xml_diff>

<commit_message>
updated for 3 tarikh
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -551,7 +551,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -718,7 +718,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>2240</v>
+        <v>2560</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -779,7 +779,9 @@
       <c r="E6" s="6">
         <v>44472</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7">
+        <v>320</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -999,7 +1001,7 @@
       </c>
       <c r="B13" s="10">
         <f>SUM(B3:B12)</f>
-        <v>5240</v>
+        <v>5560</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
@@ -1684,7 +1686,7 @@
       </c>
       <c r="F35" s="12">
         <f>SUM(F4:F34)</f>
-        <v>7773</v>
+        <v>8093</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -1752,27 +1754,27 @@
       </c>
       <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>1793.7692307692309</v>
+        <v>1867.6153846153848</v>
       </c>
       <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>797.23076923076928</v>
+        <v>830.0512820512821</v>
       </c>
       <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>797.23076923076928</v>
+        <v>830.0512820512821</v>
       </c>
       <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>797.23076923076928</v>
+        <v>830.0512820512821</v>
       </c>
       <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>597.92307692307691</v>
+        <v>622.53846153846155</v>
       </c>
       <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>797.23076923076928</v>
+        <v>830.0512820512821</v>
       </c>
       <c r="Q36" s="4">
         <f>Q35*B38</f>
@@ -1780,15 +1782,15 @@
       </c>
       <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>797.23076923076928</v>
+        <v>830.0512820512821</v>
       </c>
       <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>597.92307692307691</v>
+        <v>622.53846153846155</v>
       </c>
       <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>797.23076923076928</v>
+        <v>830.0512820512821</v>
       </c>
       <c r="U36" s="8"/>
     </row>
@@ -1805,27 +1807,27 @@
       <c r="J37" s="4"/>
       <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>1206.2307692307691</v>
+        <v>1132.3846153846152</v>
       </c>
       <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>-797.23076923076928</v>
+        <v>-830.0512820512821</v>
       </c>
       <c r="M37" s="21">
         <f>B9-M36</f>
-        <v>-797.23076923076928</v>
+        <v>-830.0512820512821</v>
       </c>
       <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>-797.23076923076928</v>
+        <v>-830.0512820512821</v>
       </c>
       <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>1642.0769230769231</v>
+        <v>1937.4615384615386</v>
       </c>
       <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>-797.23076923076928</v>
+        <v>-830.0512820512821</v>
       </c>
       <c r="Q37" s="17">
         <f>B8-Q36</f>
@@ -1833,15 +1835,15 @@
       </c>
       <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>-797.23076923076928</v>
+        <v>-830.0512820512821</v>
       </c>
       <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>-597.92307692307691</v>
+        <v>-622.53846153846155</v>
       </c>
       <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>-797.23076923076928</v>
+        <v>-830.0512820512821</v>
       </c>
       <c r="U37" s="8"/>
     </row>
@@ -1851,7 +1853,7 @@
       </c>
       <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>199.30769230769232</v>
+        <v>207.51282051282053</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>

</xml_diff>

<commit_message>
update for 3 tarikh again
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -551,7 +551,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -562,7 +562,7 @@
   <dimension ref="A1:AC104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -663,7 +663,9 @@
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4">
+        <v>2000</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="6">
@@ -788,19 +790,39 @@
       <c r="J6" s="6">
         <v>44472</v>
       </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
+      <c r="K6" s="4">
+        <v>3</v>
+      </c>
+      <c r="L6" s="4">
+        <v>2</v>
+      </c>
+      <c r="M6" s="4">
+        <v>2</v>
+      </c>
+      <c r="N6" s="4">
+        <v>2</v>
+      </c>
+      <c r="O6" s="4">
+        <v>2</v>
+      </c>
+      <c r="P6" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>0</v>
+      </c>
+      <c r="R6" s="4">
+        <v>2</v>
+      </c>
+      <c r="S6" s="4">
+        <v>2</v>
+      </c>
+      <c r="T6" s="4">
+        <v>2</v>
+      </c>
       <c r="U6" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:24">
@@ -1001,7 +1023,7 @@
       </c>
       <c r="B13" s="10">
         <f>SUM(B3:B12)</f>
-        <v>5560</v>
+        <v>7560</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
@@ -1159,7 +1181,7 @@
       </c>
       <c r="B18" s="11">
         <f>B13-F35</f>
-        <v>-2533</v>
+        <v>-533</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1696,27 +1718,27 @@
       </c>
       <c r="K35" s="14">
         <f>SUM(K4:K34)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="L35" s="14">
         <f>SUM(L4:L34)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M35" s="14">
         <f t="shared" ref="M35:T35" si="2">SUM(M4:M34)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N35" s="14">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O35" s="14">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q35" s="14">
         <f t="shared" si="2"/>
@@ -1724,19 +1746,19 @@
       </c>
       <c r="R35" s="14">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S35" s="14">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T35" s="14">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="U35" s="15">
         <f>SUM(U4:U34)</f>
-        <v>39</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:21">
@@ -1754,27 +1776,27 @@
       </c>
       <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>1867.6153846153848</v>
+        <v>1674.4137931034484</v>
       </c>
       <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>830.0512820512821</v>
+        <v>837.20689655172418</v>
       </c>
       <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>830.0512820512821</v>
+        <v>837.20689655172418</v>
       </c>
       <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>830.0512820512821</v>
+        <v>837.20689655172418</v>
       </c>
       <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>622.53846153846155</v>
+        <v>697.67241379310349</v>
       </c>
       <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>830.0512820512821</v>
+        <v>837.20689655172418</v>
       </c>
       <c r="Q36" s="4">
         <f>Q35*B38</f>
@@ -1782,15 +1804,15 @@
       </c>
       <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>830.0512820512821</v>
+        <v>837.20689655172418</v>
       </c>
       <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>622.53846153846155</v>
+        <v>697.67241379310349</v>
       </c>
       <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>830.0512820512821</v>
+        <v>837.20689655172418</v>
       </c>
       <c r="U36" s="8"/>
     </row>
@@ -1807,27 +1829,27 @@
       <c r="J37" s="4"/>
       <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>1132.3846153846152</v>
+        <v>1325.5862068965516</v>
       </c>
       <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>-830.0512820512821</v>
+        <v>1162.7931034482758</v>
       </c>
       <c r="M37" s="21">
         <f>B9-M36</f>
-        <v>-830.0512820512821</v>
+        <v>-837.20689655172418</v>
       </c>
       <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>-830.0512820512821</v>
+        <v>-837.20689655172418</v>
       </c>
       <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>1937.4615384615386</v>
+        <v>1862.3275862068965</v>
       </c>
       <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>-830.0512820512821</v>
+        <v>-837.20689655172418</v>
       </c>
       <c r="Q37" s="17">
         <f>B8-Q36</f>
@@ -1835,15 +1857,15 @@
       </c>
       <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>-830.0512820512821</v>
+        <v>-837.20689655172418</v>
       </c>
       <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>-622.53846153846155</v>
+        <v>-697.67241379310349</v>
       </c>
       <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>-830.0512820512821</v>
+        <v>-837.20689655172418</v>
       </c>
       <c r="U37" s="8"/>
     </row>
@@ -1853,7 +1875,7 @@
       </c>
       <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>207.51282051282053</v>
+        <v>139.5344827586207</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>

</xml_diff>

<commit_message>
something changed in the excel file
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>Meal list</t>
   </si>
@@ -92,9 +92,6 @@
     <t xml:space="preserve">     </t>
   </si>
   <si>
-    <t>Jahid2</t>
-  </si>
-  <si>
     <t>Gopal</t>
   </si>
   <si>
@@ -106,12 +103,24 @@
   <si>
     <t>Shovon</t>
   </si>
+  <si>
+    <t>lunch</t>
+  </si>
+  <si>
+    <t>dinner</t>
+  </si>
+  <si>
+    <t>total in day</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,14 +177,24 @@
       <name val="Roboto"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -232,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -269,7 +288,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -279,11 +297,408 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="55">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -551,7 +966,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -561,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="H7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z8" sqref="Z8:Z34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -574,16 +989,17 @@
     <col min="10" max="10" width="12" customWidth="1"/>
     <col min="20" max="20" width="12.28515625" customWidth="1"/>
     <col min="21" max="21" width="14.42578125" customWidth="1"/>
+    <col min="27" max="27" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="21">
+    <row r="1" spans="1:27" ht="21">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="1"/>
       <c r="U1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="20.25">
+    <row r="2" spans="1:27" ht="20.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -594,33 +1010,33 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-    </row>
-    <row r="3" spans="1:24" ht="18">
+      <c r="K2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+    </row>
+    <row r="3" spans="1:27" ht="18">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="22"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -641,7 +1057,7 @@
         <v>5</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>6</v>
@@ -650,7 +1066,7 @@
         <v>7</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>13</v>
@@ -658,8 +1074,17 @@
       <c r="U3" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="Y3" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z3" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA3" s="24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -714,8 +1139,21 @@
         <f>SUM(K4:T4)</f>
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="X4" s="23">
+        <v>44470</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="27">
+        <f>Y4+Z4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -770,8 +1208,21 @@
         <f t="shared" ref="U5:U7" si="0">SUM(K5:T5)</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="X5" s="23">
+        <v>44471</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="27">
+        <f t="shared" ref="AA5:AA34" si="1">Y5+Z5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -824,10 +1275,23 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="X6" s="23">
+        <v>44472</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -835,29 +1299,64 @@
       <c r="E7" s="6">
         <v>44473</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7">
+        <v>1245</v>
+      </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="6">
         <v>44473</v>
       </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
+      <c r="K7" s="4">
+        <v>2</v>
+      </c>
+      <c r="L7" s="4">
+        <v>2</v>
+      </c>
+      <c r="M7" s="9">
+        <v>2</v>
+      </c>
+      <c r="N7" s="4">
+        <v>2</v>
+      </c>
+      <c r="O7" s="4">
+        <v>2</v>
+      </c>
+      <c r="P7" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>0</v>
+      </c>
+      <c r="R7" s="9">
+        <v>2</v>
+      </c>
+      <c r="S7" s="4">
+        <v>2</v>
+      </c>
+      <c r="T7" s="4">
+        <v>2</v>
+      </c>
       <c r="U7" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24">
+        <v>18</v>
+      </c>
+      <c r="X7" s="23">
+        <v>44473</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>-1</v>
+      </c>
+      <c r="AA7" s="27">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -885,11 +1384,24 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="8">
-        <f t="shared" ref="U8:U34" si="1">SUM(K8:T8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24">
+        <f t="shared" ref="U8:U34" si="2">SUM(K8:T8)</f>
+        <v>0</v>
+      </c>
+      <c r="X8" s="23">
+        <v>44474</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -917,11 +1429,24 @@
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X9" s="23">
+        <v>44475</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:27">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -949,15 +1474,30 @@
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X10" s="23">
+        <v>44476</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:27">
       <c r="A11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="B11" s="4">
+        <v>2000</v>
+      </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="6">
@@ -981,11 +1521,24 @@
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X11" s="23">
+        <v>44477</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:27">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1013,21 +1566,34 @@
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
       <c r="U12" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X12" s="23">
+        <v>44478</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="18">
+    <row r="13" spans="1:27" ht="18">
       <c r="A13" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="10">
         <f>SUM(B3:B12)</f>
-        <v>7560</v>
+        <v>8560</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="6">
         <v>44479</v>
@@ -1050,12 +1616,24 @@
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
       <c r="U13" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X13" s="23">
+        <v>44479</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X13" s="19"/>
-    </row>
-    <row r="14" spans="1:24">
+    </row>
+    <row r="14" spans="1:27">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1081,11 +1659,24 @@
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
       <c r="U14" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X14" s="23">
+        <v>44480</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:27">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1111,11 +1702,24 @@
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
       <c r="U15" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X15" s="23">
+        <v>44481</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:27">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1141,11 +1745,24 @@
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
       <c r="U16" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X16" s="23">
+        <v>44482</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:27">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1171,17 +1788,30 @@
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
       <c r="U17" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X17" s="23">
+        <v>44483</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15.75">
+    <row r="18" spans="1:27" ht="15.75">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="11">
         <f>B13-F35</f>
-        <v>-533</v>
+        <v>-778</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1206,11 +1836,24 @@
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
       <c r="U18" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X18" s="23">
+        <v>44484</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:27">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1236,11 +1879,24 @@
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
       <c r="U19" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X19" s="23">
+        <v>44485</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:27">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1266,11 +1922,24 @@
       <c r="S20" s="4"/>
       <c r="T20" s="4"/>
       <c r="U20" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X20" s="23">
+        <v>44486</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:27">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1298,11 +1967,24 @@
       <c r="S21" s="4"/>
       <c r="T21" s="4"/>
       <c r="U21" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X21" s="23">
+        <v>44487</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:27">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1328,11 +2010,24 @@
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
       <c r="U22" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X22" s="23">
+        <v>44488</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:27">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1358,11 +2053,24 @@
       <c r="S23" s="4"/>
       <c r="T23" s="4"/>
       <c r="U23" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X23" s="23">
+        <v>44489</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:27">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1388,11 +2096,24 @@
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
       <c r="U24" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X24" s="23">
+        <v>44490</v>
+      </c>
+      <c r="Y24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:27">
       <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
@@ -1420,11 +2141,24 @@
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
       <c r="U25" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X25" s="23">
+        <v>44491</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:27">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
         <v>19</v>
@@ -1452,11 +2186,24 @@
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
       <c r="U26" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X26" s="23">
+        <v>44492</v>
+      </c>
+      <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:27">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1482,11 +2229,24 @@
       <c r="S27" s="4"/>
       <c r="T27" s="4"/>
       <c r="U27" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X27" s="23">
+        <v>44493</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:27">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1512,11 +2272,24 @@
       <c r="S28" s="4"/>
       <c r="T28" s="4"/>
       <c r="U28" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X28" s="23">
+        <v>44494</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:27">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1542,11 +2315,24 @@
       <c r="S29" s="4"/>
       <c r="T29" s="4"/>
       <c r="U29" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X29" s="23">
+        <v>44495</v>
+      </c>
+      <c r="Y29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:27">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1574,11 +2360,24 @@
       <c r="S30" s="4"/>
       <c r="T30" s="4"/>
       <c r="U30" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X30" s="23">
+        <v>44496</v>
+      </c>
+      <c r="Y30">
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:27">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1604,11 +2403,24 @@
       <c r="S31" s="4"/>
       <c r="T31" s="4"/>
       <c r="U31" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X31" s="23">
+        <v>44497</v>
+      </c>
+      <c r="Y31">
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:27">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1634,11 +2446,24 @@
       <c r="S32" s="4"/>
       <c r="T32" s="4"/>
       <c r="U32" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X32" s="23">
+        <v>44498</v>
+      </c>
+      <c r="Y32">
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:27">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1664,11 +2489,24 @@
       <c r="S33" s="4"/>
       <c r="T33" s="4"/>
       <c r="U33" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X33" s="23">
+        <v>44499</v>
+      </c>
+      <c r="Y33">
+        <v>0</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:27">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1694,11 +2532,24 @@
       <c r="S34" s="4"/>
       <c r="T34" s="4"/>
       <c r="U34" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X34" s="23">
+        <v>44500</v>
+      </c>
+      <c r="Y34">
+        <v>0</v>
+      </c>
+      <c r="Z34">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="18">
+    <row r="35" spans="1:27" ht="18.75">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1708,7 +2559,7 @@
       </c>
       <c r="F35" s="12">
         <f>SUM(F4:F34)</f>
-        <v>8093</v>
+        <v>9338</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -1718,50 +2569,65 @@
       </c>
       <c r="K35" s="14">
         <f>SUM(K4:K34)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L35" s="14">
         <f>SUM(L4:L34)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M35" s="14">
-        <f t="shared" ref="M35:T35" si="2">SUM(M4:M34)</f>
-        <v>6</v>
+        <f t="shared" ref="M35:T35" si="3">SUM(M4:M34)</f>
+        <v>8</v>
       </c>
       <c r="N35" s="14">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="O35" s="14">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>7</v>
       </c>
       <c r="P35" s="14">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="Q35" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R35" s="14">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="S35" s="14">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>7</v>
       </c>
       <c r="T35" s="14">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="U35" s="15">
         <f>SUM(U4:U34)</f>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21">
+        <v>76</v>
+      </c>
+      <c r="X35" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y35" s="26">
+        <f>SUM(Y4:Y34)</f>
+        <v>0</v>
+      </c>
+      <c r="Z35" s="26">
+        <f>SUM(Z4:Z34)</f>
+        <v>-1</v>
+      </c>
+      <c r="AA35" s="26">
+        <f>SUM(AA4:AA34)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1776,27 +2642,27 @@
       </c>
       <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>1674.4137931034484</v>
+        <v>1720.1578947368421</v>
       </c>
       <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>837.20689655172418</v>
+        <v>982.9473684210526</v>
       </c>
       <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>837.20689655172418</v>
+        <v>982.9473684210526</v>
       </c>
       <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>837.20689655172418</v>
+        <v>982.9473684210526</v>
       </c>
       <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>697.67241379310349</v>
+        <v>860.07894736842104</v>
       </c>
       <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>837.20689655172418</v>
+        <v>982.9473684210526</v>
       </c>
       <c r="Q36" s="4">
         <f>Q35*B38</f>
@@ -1804,19 +2670,19 @@
       </c>
       <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>837.20689655172418</v>
+        <v>982.9473684210526</v>
       </c>
       <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>697.67241379310349</v>
+        <v>860.07894736842104</v>
       </c>
       <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>837.20689655172418</v>
+        <v>982.9473684210526</v>
       </c>
       <c r="U36" s="8"/>
     </row>
-    <row r="37" spans="1:21">
+    <row r="37" spans="1:27">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1829,27 +2695,27 @@
       <c r="J37" s="4"/>
       <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>1325.5862068965516</v>
+        <v>279.84210526315792</v>
       </c>
       <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>1162.7931034482758</v>
-      </c>
-      <c r="M37" s="21">
+        <v>1017.0526315789474</v>
+      </c>
+      <c r="M37" s="20">
         <f>B9-M36</f>
-        <v>-837.20689655172418</v>
+        <v>-982.9473684210526</v>
       </c>
       <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>-837.20689655172418</v>
+        <v>-982.9473684210526</v>
       </c>
       <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>1862.3275862068965</v>
+        <v>1699.921052631579</v>
       </c>
       <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>-837.20689655172418</v>
+        <v>-982.9473684210526</v>
       </c>
       <c r="Q37" s="17">
         <f>B8-Q36</f>
@@ -1857,25 +2723,25 @@
       </c>
       <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>-837.20689655172418</v>
+        <v>-982.9473684210526</v>
       </c>
       <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>-697.67241379310349</v>
+        <v>1139.921052631579</v>
       </c>
       <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>-837.20689655172418</v>
+        <v>-982.9473684210526</v>
       </c>
       <c r="U37" s="8"/>
     </row>
-    <row r="38" spans="1:21" ht="15.75">
+    <row r="38" spans="1:27" ht="15.75">
       <c r="A38" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>139.5344827586207</v>
+        <v>122.86842105263158</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -1885,39 +2751,39 @@
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
-      <c r="K38" s="4" t="s">
+      <c r="K38" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="L38" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M38" s="9" t="s">
+      <c r="L38" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M38" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="N38" s="4" t="s">
+      <c r="N38" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="O38" s="4" t="s">
+      <c r="O38" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="P38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q38" s="4" t="s">
+      <c r="P38" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q38" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="R38" s="4" t="s">
+      <c r="R38" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="S38" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="T38" s="4" t="s">
+      <c r="S38" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="T38" s="8" t="s">
         <v>13</v>
       </c>
       <c r="U38" s="8"/>
     </row>
-    <row r="39" spans="1:21">
+    <row r="39" spans="1:27">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1942,7 +2808,7 @@
       <c r="T39" s="4"/>
       <c r="U39" s="8"/>
     </row>
-    <row r="40" spans="1:21">
+    <row r="40" spans="1:27">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1965,7 +2831,7 @@
       <c r="T40" s="4"/>
       <c r="U40" s="4"/>
     </row>
-    <row r="41" spans="1:21">
+    <row r="41" spans="1:27">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1988,7 +2854,7 @@
       <c r="T41" s="4"/>
       <c r="U41" s="4"/>
     </row>
-    <row r="42" spans="1:21">
+    <row r="42" spans="1:27">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2007,56 +2873,56 @@
       <c r="P42" s="4"/>
       <c r="Q42" s="4"/>
       <c r="R42" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S42" s="4"/>
       <c r="T42" s="4"/>
       <c r="U42" s="4"/>
     </row>
-    <row r="43" spans="1:21">
-      <c r="L43" s="20"/>
-      <c r="M43" s="20"/>
-      <c r="N43" s="20"/>
-    </row>
-    <row r="44" spans="1:21">
-      <c r="L44" s="20"/>
-      <c r="M44" s="20"/>
-      <c r="N44" s="20"/>
-    </row>
-    <row r="45" spans="1:21">
-      <c r="L45" s="20"/>
-      <c r="M45" s="20"/>
-      <c r="N45" s="20"/>
-    </row>
-    <row r="46" spans="1:21">
-      <c r="L46" s="20"/>
-      <c r="M46" s="20"/>
-      <c r="N46" s="20"/>
-    </row>
-    <row r="47" spans="1:21">
-      <c r="L47" s="20"/>
-      <c r="M47" s="20"/>
-      <c r="N47" s="20"/>
-    </row>
-    <row r="48" spans="1:21">
-      <c r="L48" s="20"/>
-      <c r="M48" s="20"/>
-      <c r="N48" s="20"/>
+    <row r="43" spans="1:27">
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
+    </row>
+    <row r="44" spans="1:27">
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+    </row>
+    <row r="45" spans="1:27">
+      <c r="L45" s="19"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="19"/>
+    </row>
+    <row r="46" spans="1:27">
+      <c r="L46" s="19"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="19"/>
+    </row>
+    <row r="47" spans="1:27">
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="19"/>
+    </row>
+    <row r="48" spans="1:27">
+      <c r="L48" s="19"/>
+      <c r="M48" s="19"/>
+      <c r="N48" s="19"/>
     </row>
     <row r="49" spans="12:14">
-      <c r="L49" s="20"/>
-      <c r="M49" s="20"/>
-      <c r="N49" s="20"/>
+      <c r="L49" s="19"/>
+      <c r="M49" s="19"/>
+      <c r="N49" s="19"/>
     </row>
     <row r="50" spans="12:14">
-      <c r="L50" s="20"/>
-      <c r="M50" s="20"/>
-      <c r="N50" s="20"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
     </row>
     <row r="51" spans="12:14">
-      <c r="L51" s="20"/>
-      <c r="M51" s="20"/>
-      <c r="N51" s="20"/>
+      <c r="L51" s="19"/>
+      <c r="M51" s="19"/>
+      <c r="N51" s="19"/>
     </row>
     <row r="104" spans="29:29">
       <c r="AC104" t="s">
@@ -2068,6 +2934,56 @@
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="K2:U2"/>
   </mergeCells>
+  <conditionalFormatting sqref="K37">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L37">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M37">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N37">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O37">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P37">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q37">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R37">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S37">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T37">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update for 5 tarikh
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -291,12 +291,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -308,326 +302,17 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <condense val="0"/>
@@ -966,7 +651,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -976,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z8" sqref="Z8:Z34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1010,19 +695,19 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
+      <c r="K2" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
     </row>
     <row r="3" spans="1:27" ht="18">
       <c r="A3" s="4" t="s">
@@ -1033,10 +718,10 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="21"/>
+      <c r="F3" s="26"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1074,13 +759,13 @@
       <c r="U3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="Y3" s="25" t="s">
+      <c r="Y3" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="Z3" s="25" t="s">
+      <c r="Z3" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="AA3" s="24" t="s">
+      <c r="AA3" s="22" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1139,7 +824,7 @@
         <f>SUM(K4:T4)</f>
         <v>19</v>
       </c>
-      <c r="X4" s="23">
+      <c r="X4" s="21">
         <v>44470</v>
       </c>
       <c r="Y4">
@@ -1148,7 +833,7 @@
       <c r="Z4">
         <v>0</v>
       </c>
-      <c r="AA4" s="27">
+      <c r="AA4" s="25">
         <f>Y4+Z4</f>
         <v>0</v>
       </c>
@@ -1208,7 +893,7 @@
         <f t="shared" ref="U5:U7" si="0">SUM(K5:T5)</f>
         <v>20</v>
       </c>
-      <c r="X5" s="23">
+      <c r="X5" s="21">
         <v>44471</v>
       </c>
       <c r="Y5">
@@ -1217,7 +902,7 @@
       <c r="Z5">
         <v>0</v>
       </c>
-      <c r="AA5" s="27">
+      <c r="AA5" s="25">
         <f t="shared" ref="AA5:AA34" si="1">Y5+Z5</f>
         <v>0</v>
       </c>
@@ -1275,7 +960,7 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="X6" s="23">
+      <c r="X6" s="21">
         <v>44472</v>
       </c>
       <c r="Y6">
@@ -1284,7 +969,7 @@
       <c r="Z6">
         <v>0</v>
       </c>
-      <c r="AA6" s="27">
+      <c r="AA6" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1342,7 +1027,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="X7" s="23">
+      <c r="X7" s="21">
         <v>44473</v>
       </c>
       <c r="Y7">
@@ -1351,7 +1036,7 @@
       <c r="Z7">
         <v>-1</v>
       </c>
-      <c r="AA7" s="27">
+      <c r="AA7" s="25">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
@@ -1366,28 +1051,50 @@
       <c r="E8" s="6">
         <v>44474</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7">
+        <v>1640</v>
+      </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="6">
         <v>44474</v>
       </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
+      <c r="K8" s="4">
+        <v>2</v>
+      </c>
+      <c r="L8" s="4">
+        <v>2</v>
+      </c>
+      <c r="M8" s="9">
+        <v>2</v>
+      </c>
+      <c r="N8" s="4">
+        <v>2</v>
+      </c>
+      <c r="O8" s="4">
+        <v>2</v>
+      </c>
+      <c r="P8" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>0</v>
+      </c>
+      <c r="R8" s="4">
+        <v>2</v>
+      </c>
+      <c r="S8" s="4">
+        <v>2</v>
+      </c>
+      <c r="T8" s="4">
+        <v>2</v>
+      </c>
       <c r="U8" s="8">
         <f t="shared" ref="U8:U34" si="2">SUM(K8:T8)</f>
-        <v>0</v>
-      </c>
-      <c r="X8" s="23">
+        <v>18</v>
+      </c>
+      <c r="X8" s="21">
         <v>44474</v>
       </c>
       <c r="Y8">
@@ -1396,7 +1103,7 @@
       <c r="Z8">
         <v>0</v>
       </c>
-      <c r="AA8" s="27">
+      <c r="AA8" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1432,7 +1139,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X9" s="23">
+      <c r="X9" s="21">
         <v>44475</v>
       </c>
       <c r="Y9">
@@ -1441,7 +1148,7 @@
       <c r="Z9">
         <v>0</v>
       </c>
-      <c r="AA9" s="27">
+      <c r="AA9" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1477,7 +1184,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X10" s="23">
+      <c r="X10" s="21">
         <v>44476</v>
       </c>
       <c r="Y10">
@@ -1486,7 +1193,7 @@
       <c r="Z10">
         <v>0</v>
       </c>
-      <c r="AA10" s="27">
+      <c r="AA10" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1524,7 +1231,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X11" s="23">
+      <c r="X11" s="21">
         <v>44477</v>
       </c>
       <c r="Y11">
@@ -1533,7 +1240,7 @@
       <c r="Z11">
         <v>0</v>
       </c>
-      <c r="AA11" s="27">
+      <c r="AA11" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1569,7 +1276,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X12" s="23">
+      <c r="X12" s="21">
         <v>44478</v>
       </c>
       <c r="Y12">
@@ -1578,7 +1285,7 @@
       <c r="Z12">
         <v>0</v>
       </c>
-      <c r="AA12" s="27">
+      <c r="AA12" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1619,7 +1326,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X13" s="23">
+      <c r="X13" s="21">
         <v>44479</v>
       </c>
       <c r="Y13">
@@ -1628,7 +1335,7 @@
       <c r="Z13">
         <v>0</v>
       </c>
-      <c r="AA13" s="27">
+      <c r="AA13" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1662,7 +1369,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X14" s="23">
+      <c r="X14" s="21">
         <v>44480</v>
       </c>
       <c r="Y14">
@@ -1671,7 +1378,7 @@
       <c r="Z14">
         <v>0</v>
       </c>
-      <c r="AA14" s="27">
+      <c r="AA14" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1705,7 +1412,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X15" s="23">
+      <c r="X15" s="21">
         <v>44481</v>
       </c>
       <c r="Y15">
@@ -1714,7 +1421,7 @@
       <c r="Z15">
         <v>0</v>
       </c>
-      <c r="AA15" s="27">
+      <c r="AA15" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1748,7 +1455,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X16" s="23">
+      <c r="X16" s="21">
         <v>44482</v>
       </c>
       <c r="Y16">
@@ -1757,7 +1464,7 @@
       <c r="Z16">
         <v>0</v>
       </c>
-      <c r="AA16" s="27">
+      <c r="AA16" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1791,7 +1498,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X17" s="23">
+      <c r="X17" s="21">
         <v>44483</v>
       </c>
       <c r="Y17">
@@ -1800,7 +1507,7 @@
       <c r="Z17">
         <v>0</v>
       </c>
-      <c r="AA17" s="27">
+      <c r="AA17" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1811,7 +1518,7 @@
       </c>
       <c r="B18" s="11">
         <f>B13-F35</f>
-        <v>-778</v>
+        <v>-2418</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1839,7 +1546,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X18" s="23">
+      <c r="X18" s="21">
         <v>44484</v>
       </c>
       <c r="Y18">
@@ -1848,7 +1555,7 @@
       <c r="Z18">
         <v>0</v>
       </c>
-      <c r="AA18" s="27">
+      <c r="AA18" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1882,7 +1589,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X19" s="23">
+      <c r="X19" s="21">
         <v>44485</v>
       </c>
       <c r="Y19">
@@ -1891,7 +1598,7 @@
       <c r="Z19">
         <v>0</v>
       </c>
-      <c r="AA19" s="27">
+      <c r="AA19" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1925,7 +1632,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X20" s="23">
+      <c r="X20" s="21">
         <v>44486</v>
       </c>
       <c r="Y20">
@@ -1934,7 +1641,7 @@
       <c r="Z20">
         <v>0</v>
       </c>
-      <c r="AA20" s="27">
+      <c r="AA20" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1970,7 +1677,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X21" s="23">
+      <c r="X21" s="21">
         <v>44487</v>
       </c>
       <c r="Y21">
@@ -1979,7 +1686,7 @@
       <c r="Z21">
         <v>0</v>
       </c>
-      <c r="AA21" s="27">
+      <c r="AA21" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2013,7 +1720,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X22" s="23">
+      <c r="X22" s="21">
         <v>44488</v>
       </c>
       <c r="Y22">
@@ -2022,7 +1729,7 @@
       <c r="Z22">
         <v>0</v>
       </c>
-      <c r="AA22" s="27">
+      <c r="AA22" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2056,7 +1763,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X23" s="23">
+      <c r="X23" s="21">
         <v>44489</v>
       </c>
       <c r="Y23">
@@ -2065,7 +1772,7 @@
       <c r="Z23">
         <v>0</v>
       </c>
-      <c r="AA23" s="27">
+      <c r="AA23" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2099,7 +1806,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X24" s="23">
+      <c r="X24" s="21">
         <v>44490</v>
       </c>
       <c r="Y24">
@@ -2108,7 +1815,7 @@
       <c r="Z24">
         <v>0</v>
       </c>
-      <c r="AA24" s="27">
+      <c r="AA24" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2144,7 +1851,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X25" s="23">
+      <c r="X25" s="21">
         <v>44491</v>
       </c>
       <c r="Y25">
@@ -2153,7 +1860,7 @@
       <c r="Z25">
         <v>0</v>
       </c>
-      <c r="AA25" s="27">
+      <c r="AA25" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2189,7 +1896,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X26" s="23">
+      <c r="X26" s="21">
         <v>44492</v>
       </c>
       <c r="Y26">
@@ -2198,7 +1905,7 @@
       <c r="Z26">
         <v>0</v>
       </c>
-      <c r="AA26" s="27">
+      <c r="AA26" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2232,7 +1939,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X27" s="23">
+      <c r="X27" s="21">
         <v>44493</v>
       </c>
       <c r="Y27">
@@ -2241,7 +1948,7 @@
       <c r="Z27">
         <v>0</v>
       </c>
-      <c r="AA27" s="27">
+      <c r="AA27" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2275,7 +1982,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X28" s="23">
+      <c r="X28" s="21">
         <v>44494</v>
       </c>
       <c r="Y28">
@@ -2284,7 +1991,7 @@
       <c r="Z28">
         <v>0</v>
       </c>
-      <c r="AA28" s="27">
+      <c r="AA28" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2318,7 +2025,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X29" s="23">
+      <c r="X29" s="21">
         <v>44495</v>
       </c>
       <c r="Y29">
@@ -2327,7 +2034,7 @@
       <c r="Z29">
         <v>0</v>
       </c>
-      <c r="AA29" s="27">
+      <c r="AA29" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2363,7 +2070,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X30" s="23">
+      <c r="X30" s="21">
         <v>44496</v>
       </c>
       <c r="Y30">
@@ -2372,7 +2079,7 @@
       <c r="Z30">
         <v>0</v>
       </c>
-      <c r="AA30" s="27">
+      <c r="AA30" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2406,7 +2113,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X31" s="23">
+      <c r="X31" s="21">
         <v>44497</v>
       </c>
       <c r="Y31">
@@ -2415,7 +2122,7 @@
       <c r="Z31">
         <v>0</v>
       </c>
-      <c r="AA31" s="27">
+      <c r="AA31" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2449,7 +2156,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X32" s="23">
+      <c r="X32" s="21">
         <v>44498</v>
       </c>
       <c r="Y32">
@@ -2458,7 +2165,7 @@
       <c r="Z32">
         <v>0</v>
       </c>
-      <c r="AA32" s="27">
+      <c r="AA32" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2492,7 +2199,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X33" s="23">
+      <c r="X33" s="21">
         <v>44499</v>
       </c>
       <c r="Y33">
@@ -2501,7 +2208,7 @@
       <c r="Z33">
         <v>0</v>
       </c>
-      <c r="AA33" s="27">
+      <c r="AA33" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2535,7 +2242,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X34" s="23">
+      <c r="X34" s="21">
         <v>44500</v>
       </c>
       <c r="Y34">
@@ -2544,7 +2251,7 @@
       <c r="Z34">
         <v>0</v>
       </c>
-      <c r="AA34" s="27">
+      <c r="AA34" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2559,7 +2266,7 @@
       </c>
       <c r="F35" s="12">
         <f>SUM(F4:F34)</f>
-        <v>9338</v>
+        <v>10978</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -2569,27 +2276,27 @@
       </c>
       <c r="K35" s="14">
         <f>SUM(K4:K34)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L35" s="14">
         <f>SUM(L4:L34)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M35" s="14">
         <f t="shared" ref="M35:T35" si="3">SUM(M4:M34)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N35" s="14">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="O35" s="14">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q35" s="14">
         <f t="shared" si="3"/>
@@ -2597,32 +2304,32 @@
       </c>
       <c r="R35" s="14">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="S35" s="14">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="T35" s="14">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="U35" s="15">
         <f>SUM(U4:U34)</f>
-        <v>76</v>
-      </c>
-      <c r="X35" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="X35" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="Y35" s="26">
+      <c r="Y35" s="24">
         <f>SUM(Y4:Y34)</f>
         <v>0</v>
       </c>
-      <c r="Z35" s="26">
+      <c r="Z35" s="24">
         <f>SUM(Z4:Z34)</f>
         <v>-1</v>
       </c>
-      <c r="AA35" s="26">
+      <c r="AA35" s="24">
         <f>SUM(AA4:AA34)</f>
         <v>-1</v>
       </c>
@@ -2642,27 +2349,27 @@
       </c>
       <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>1720.1578947368421</v>
+        <v>1868.5957446808511</v>
       </c>
       <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>982.9473684210526</v>
+        <v>1167.872340425532</v>
       </c>
       <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>982.9473684210526</v>
+        <v>1167.872340425532</v>
       </c>
       <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>982.9473684210526</v>
+        <v>1167.872340425532</v>
       </c>
       <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>860.07894736842104</v>
+        <v>1051.0851063829787</v>
       </c>
       <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>982.9473684210526</v>
+        <v>1167.872340425532</v>
       </c>
       <c r="Q36" s="4">
         <f>Q35*B38</f>
@@ -2670,15 +2377,15 @@
       </c>
       <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>982.9473684210526</v>
+        <v>1167.872340425532</v>
       </c>
       <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>860.07894736842104</v>
+        <v>1051.0851063829787</v>
       </c>
       <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>982.9473684210526</v>
+        <v>1167.872340425532</v>
       </c>
       <c r="U36" s="8"/>
     </row>
@@ -2695,27 +2402,27 @@
       <c r="J37" s="4"/>
       <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>279.84210526315792</v>
+        <v>131.40425531914889</v>
       </c>
       <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>1017.0526315789474</v>
+        <v>832.127659574468</v>
       </c>
       <c r="M37" s="20">
         <f>B9-M36</f>
-        <v>-982.9473684210526</v>
+        <v>-1167.872340425532</v>
       </c>
       <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>-982.9473684210526</v>
+        <v>-1167.872340425532</v>
       </c>
       <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>1699.921052631579</v>
+        <v>1508.9148936170213</v>
       </c>
       <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>-982.9473684210526</v>
+        <v>-1167.872340425532</v>
       </c>
       <c r="Q37" s="17">
         <f>B8-Q36</f>
@@ -2723,15 +2430,15 @@
       </c>
       <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>-982.9473684210526</v>
+        <v>-1167.872340425532</v>
       </c>
       <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>1139.921052631579</v>
+        <v>948.91489361702133</v>
       </c>
       <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>-982.9473684210526</v>
+        <v>-1167.872340425532</v>
       </c>
       <c r="U37" s="8"/>
     </row>
@@ -2741,7 +2448,7 @@
       </c>
       <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>122.86842105263158</v>
+        <v>116.78723404255319</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -2935,47 +2642,47 @@
     <mergeCell ref="K2:U2"/>
   </mergeCells>
   <conditionalFormatting sqref="K37">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L37">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M37">
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N37">
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O37">
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P37">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q37">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R37">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S37">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update form 6 tairkh
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>Meal list</t>
   </si>
@@ -98,9 +98,6 @@
     <t xml:space="preserve">                                      </t>
   </si>
   <si>
-    <t xml:space="preserve">         </t>
-  </si>
-  <si>
     <t>Shovon</t>
   </si>
   <si>
@@ -114,13 +111,25 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>Paid from prev month due</t>
+  </si>
+  <si>
+    <t>Prev Due to meal ( collected )</t>
+  </si>
+  <si>
+    <t>Total Balance of due from prev month</t>
+  </si>
+  <si>
+    <t>rakib vai</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,8 +209,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +226,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -251,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -302,6 +323,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -661,19 +688,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
     <col min="20" max="20" width="12.28515625" customWidth="1"/>
     <col min="21" max="21" width="14.42578125" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" customWidth="1"/>
     <col min="27" max="27" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -683,31 +713,41 @@
       </c>
       <c r="M1" s="1"/>
       <c r="U1" s="2"/>
+      <c r="V1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="2" spans="1:27" ht="20.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
+      <c r="K2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:27" ht="18">
       <c r="A3" s="4" t="s">
@@ -718,10 +758,10 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="26"/>
+      <c r="F3" s="30"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -751,7 +791,7 @@
         <v>7</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>13</v>
@@ -760,13 +800,13 @@
         <v>8</v>
       </c>
       <c r="Y3" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z3" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="Z3" s="23" t="s">
+      <c r="AA3" s="22" t="s">
         <v>27</v>
-      </c>
-      <c r="AA3" s="22" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -774,10 +814,14 @@
         <v>2</v>
       </c>
       <c r="B4" s="4">
-        <v>2000</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+        <v>2909</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>409</v>
+      </c>
       <c r="E4" s="6">
         <v>44470</v>
       </c>
@@ -978,8 +1022,12 @@
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="B7" s="4">
+        <v>2000</v>
+      </c>
+      <c r="C7" s="4">
+        <v>93</v>
+      </c>
       <c r="D7" s="4"/>
       <c r="E7" s="6">
         <v>44473</v>
@@ -1070,7 +1118,7 @@
         <v>2</v>
       </c>
       <c r="N8" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O8" s="4">
         <v>2</v>
@@ -1092,7 +1140,7 @@
       </c>
       <c r="U8" s="8">
         <f t="shared" ref="U8:U34" si="2">SUM(K8:T8)</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="X8" s="21">
         <v>44474</v>
@@ -1118,26 +1166,48 @@
       <c r="E9" s="6">
         <v>44475</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="29">
+        <v>2123</v>
+      </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="6">
         <v>44475</v>
       </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
+      <c r="K9" s="4">
+        <v>2</v>
+      </c>
+      <c r="L9" s="4">
+        <v>2</v>
+      </c>
+      <c r="M9" s="9">
+        <v>2</v>
+      </c>
+      <c r="N9" s="4">
+        <v>3</v>
+      </c>
+      <c r="O9" s="4">
+        <v>2</v>
+      </c>
+      <c r="P9" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>0</v>
+      </c>
+      <c r="R9" s="4">
+        <v>2</v>
+      </c>
+      <c r="S9" s="4">
+        <v>2</v>
+      </c>
+      <c r="T9" s="4">
+        <v>2</v>
+      </c>
       <c r="U9" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="X9" s="21">
         <v>44475</v>
@@ -1200,7 +1270,7 @@
     </row>
     <row r="11" spans="1:27">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="4">
         <v>2000</v>
@@ -1249,8 +1319,12 @@
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="4">
+        <v>1924</v>
+      </c>
+      <c r="C12" s="4">
+        <v>476</v>
+      </c>
       <c r="D12" s="4"/>
       <c r="E12" s="6">
         <v>44478</v>
@@ -1296,11 +1370,15 @@
       </c>
       <c r="B13" s="10">
         <f>SUM(B3:B12)</f>
-        <v>8560</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4" t="s">
-        <v>24</v>
+        <v>13393</v>
+      </c>
+      <c r="C13" s="26">
+        <f>SUM(C3:C12)</f>
+        <v>569</v>
+      </c>
+      <c r="D13" s="26">
+        <f>SUM(D3:D12)</f>
+        <v>409</v>
       </c>
       <c r="E13" s="6">
         <v>44479</v>
@@ -1383,11 +1461,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" ht="15.75">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="27">
+        <f>C13-D13</f>
+        <v>160</v>
+      </c>
       <c r="E15" s="6">
         <v>44481</v>
       </c>
@@ -1518,7 +1601,7 @@
       </c>
       <c r="B18" s="11">
         <f>B13-F35</f>
-        <v>-2418</v>
+        <v>292</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2266,7 +2349,7 @@
       </c>
       <c r="F35" s="12">
         <f>SUM(F4:F34)</f>
-        <v>10978</v>
+        <v>13101</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -2276,27 +2359,27 @@
       </c>
       <c r="K35" s="14">
         <f>SUM(K4:K34)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L35" s="14">
         <f>SUM(L4:L34)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M35" s="14">
         <f t="shared" ref="M35:T35" si="3">SUM(M4:M34)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N35" s="14">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="O35" s="14">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q35" s="14">
         <f t="shared" si="3"/>
@@ -2304,22 +2387,22 @@
       </c>
       <c r="R35" s="14">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="S35" s="14">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="T35" s="14">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="U35" s="15">
         <f>SUM(U4:U34)</f>
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="X35" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y35" s="24">
         <f>SUM(Y4:Y34)</f>
@@ -2349,27 +2432,27 @@
       </c>
       <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>1868.5957446808511</v>
+        <v>2105.5178571428573</v>
       </c>
       <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>1167.872340425532</v>
+        <v>1403.6785714285716</v>
       </c>
       <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>1167.872340425532</v>
+        <v>1403.6785714285716</v>
       </c>
       <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>1167.872340425532</v>
+        <v>1403.6785714285716</v>
       </c>
       <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>1051.0851063829787</v>
+        <v>1286.7053571428571</v>
       </c>
       <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>1167.872340425532</v>
+        <v>1403.6785714285716</v>
       </c>
       <c r="Q36" s="4">
         <f>Q35*B38</f>
@@ -2377,15 +2460,15 @@
       </c>
       <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>1167.872340425532</v>
+        <v>1403.6785714285716</v>
       </c>
       <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>1051.0851063829787</v>
+        <v>1286.7053571428571</v>
       </c>
       <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>1167.872340425532</v>
+        <v>1403.6785714285716</v>
       </c>
       <c r="U36" s="8"/>
     </row>
@@ -2402,27 +2485,27 @@
       <c r="J37" s="4"/>
       <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>131.40425531914889</v>
+        <v>-105.51785714285734</v>
       </c>
       <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>832.127659574468</v>
+        <v>1505.3214285714284</v>
       </c>
       <c r="M37" s="20">
         <f>B9-M36</f>
-        <v>-1167.872340425532</v>
+        <v>-1403.6785714285716</v>
       </c>
       <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>-1167.872340425532</v>
+        <v>-1403.6785714285716</v>
       </c>
       <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>1508.9148936170213</v>
+        <v>1273.2946428571429</v>
       </c>
       <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>-1167.872340425532</v>
+        <v>596.32142857142844</v>
       </c>
       <c r="Q37" s="17">
         <f>B8-Q36</f>
@@ -2430,15 +2513,15 @@
       </c>
       <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>-1167.872340425532</v>
+        <v>-1403.6785714285716</v>
       </c>
       <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>948.91489361702133</v>
+        <v>713.29464285714289</v>
       </c>
       <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>-1167.872340425532</v>
+        <v>520.32142857142844</v>
       </c>
       <c r="U37" s="8"/>
     </row>
@@ -2448,7 +2531,7 @@
       </c>
       <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>116.78723404255319</v>
+        <v>116.97321428571429</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -2483,7 +2566,7 @@
         <v>7</v>
       </c>
       <c r="S38" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="T38" s="8" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
updated for 11 tarikh
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -132,7 +132,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +218,18 @@
       <color theme="5" tint="-0.249977111117893"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -275,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -336,6 +348,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -681,7 +699,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -691,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -726,10 +744,10 @@
     <row r="2" spans="1:27" ht="20.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="33" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="4"/>
@@ -1235,8 +1253,12 @@
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="B10" s="4">
+        <v>1623</v>
+      </c>
+      <c r="C10" s="4">
+        <v>977</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="6">
         <v>44476</v>
@@ -1301,7 +1323,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="4">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1442,11 +1464,11 @@
       </c>
       <c r="B13" s="10">
         <f>SUM(B3:B12)</f>
-        <v>15969</v>
+        <v>17607</v>
       </c>
       <c r="C13" s="26">
         <f>SUM(C3:C12)</f>
-        <v>569</v>
+        <v>1546</v>
       </c>
       <c r="D13" s="26">
         <f>SUM(D3:D12)</f>
@@ -1520,26 +1542,48 @@
       <c r="E14" s="6">
         <v>44480</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7">
+        <v>100</v>
+      </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="6">
         <v>44480</v>
       </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
+        <v>2</v>
+      </c>
+      <c r="M14" s="9">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>1</v>
+      </c>
+      <c r="O14" s="4">
+        <v>2</v>
+      </c>
+      <c r="P14" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>1</v>
+      </c>
+      <c r="R14" s="4">
+        <v>2</v>
+      </c>
+      <c r="S14" s="4">
+        <v>2</v>
+      </c>
+      <c r="T14" s="4">
+        <v>3</v>
+      </c>
       <c r="U14" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="X14" s="21">
         <v>44480</v>
@@ -1563,7 +1607,7 @@
       </c>
       <c r="D15" s="27">
         <f>C13-D13</f>
-        <v>160</v>
+        <v>1137</v>
       </c>
       <c r="E15" s="6">
         <v>44481</v>
@@ -1695,7 +1739,7 @@
       </c>
       <c r="B18" s="11">
         <f>B13-F35</f>
-        <v>581</v>
+        <v>2119</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2443,7 +2487,7 @@
       </c>
       <c r="F35" s="12">
         <f>SUM(F4:F34)</f>
-        <v>15388</v>
+        <v>15488</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -2457,7 +2501,7 @@
       </c>
       <c r="L35" s="14">
         <f>SUM(L4:L34)</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M35" s="14">
         <f t="shared" ref="M35:T35" si="3">SUM(M4:M34)</f>
@@ -2465,35 +2509,35 @@
       </c>
       <c r="N35" s="14">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O35" s="14">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="Q35" s="14">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R35" s="14">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="S35" s="14">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="T35" s="14">
         <f t="shared" si="3"/>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="U35" s="15">
         <f>SUM(U4:U34)</f>
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="X35" s="24" t="s">
         <v>28</v>
@@ -2526,43 +2570,43 @@
       </c>
       <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>1933.1658291457288</v>
+        <v>1809.3457943925234</v>
       </c>
       <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>1546.532663316583</v>
+        <v>1592.2242990654206</v>
       </c>
       <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>1546.532663316583</v>
+        <v>1447.4766355140187</v>
       </c>
       <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>2010.492462311558</v>
+        <v>1954.0934579439252</v>
       </c>
       <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>1469.2060301507538</v>
+        <v>1519.8504672897197</v>
       </c>
       <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>1546.532663316583</v>
+        <v>1592.2242990654206</v>
       </c>
       <c r="Q36" s="4">
         <f>Q35*B38</f>
-        <v>541.286432160804</v>
+        <v>578.99065420560748</v>
       </c>
       <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>1546.532663316583</v>
+        <v>1592.2242990654206</v>
       </c>
       <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>1391.8793969849248</v>
+        <v>1447.4766355140187</v>
       </c>
       <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>1855.8391959798996</v>
+        <v>1954.0934579439252</v>
       </c>
       <c r="U36" s="8"/>
     </row>
@@ -2579,43 +2623,43 @@
       <c r="J37" s="4"/>
       <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>66.834170854271179</v>
+        <v>190.65420560747657</v>
       </c>
       <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>1362.467336683417</v>
+        <v>1316.7757009345794</v>
       </c>
       <c r="M37" s="20">
         <f>B9-M36</f>
-        <v>-1546.532663316583</v>
+        <v>-1447.4766355140187</v>
       </c>
       <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>-2010.492462311558</v>
+        <v>-1954.0934579439252</v>
       </c>
       <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>1090.7939698492462</v>
+        <v>1040.1495327102803</v>
       </c>
       <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>453.46733668341699</v>
+        <v>407.77570093457939</v>
       </c>
       <c r="Q37" s="17">
         <f>B8-Q36</f>
-        <v>1458.713567839196</v>
+        <v>1421.0093457943926</v>
       </c>
       <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>-1546.532663316583</v>
+        <v>30.77570093457939</v>
       </c>
       <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>608.12060301507518</v>
+        <v>567.52336448598135</v>
       </c>
       <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>644.16080402010039</v>
+        <v>545.90654205607484</v>
       </c>
       <c r="U37" s="8"/>
     </row>
@@ -2625,7 +2669,7 @@
       </c>
       <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>77.326633165829151</v>
+        <v>72.373831775700936</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>

</xml_diff>

<commit_message>
updated for 12 tarikh
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -344,16 +344,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -699,7 +699,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -709,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -744,10 +744,10 @@
     <row r="2" spans="1:27" ht="20.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="31" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="4"/>
@@ -756,19 +756,19 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
+      <c r="K2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2">
         <v>10</v>
       </c>
@@ -782,10 +782,10 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="30"/>
+      <c r="F3" s="32"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1612,26 +1612,48 @@
       <c r="E15" s="6">
         <v>44481</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="7">
+        <v>1400</v>
+      </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="6">
         <v>44481</v>
       </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <v>2</v>
+      </c>
+      <c r="M15" s="9">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>2</v>
+      </c>
+      <c r="O15" s="4">
+        <v>2</v>
+      </c>
+      <c r="P15" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>2</v>
+      </c>
+      <c r="R15" s="4">
+        <v>2</v>
+      </c>
+      <c r="S15" s="4">
+        <v>0</v>
+      </c>
+      <c r="T15" s="4">
+        <v>2</v>
+      </c>
       <c r="U15" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="X15" s="21">
         <v>44481</v>
@@ -1739,7 +1761,7 @@
       </c>
       <c r="B18" s="11">
         <f>B13-F35</f>
-        <v>2119</v>
+        <v>719</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2487,7 +2509,7 @@
       </c>
       <c r="F35" s="12">
         <f>SUM(F4:F34)</f>
-        <v>15488</v>
+        <v>16888</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -2501,7 +2523,7 @@
       </c>
       <c r="L35" s="14">
         <f>SUM(L4:L34)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M35" s="14">
         <f t="shared" ref="M35:T35" si="3">SUM(M4:M34)</f>
@@ -2509,23 +2531,23 @@
       </c>
       <c r="N35" s="14">
         <f t="shared" si="3"/>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="O35" s="14">
         <f t="shared" si="3"/>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="Q35" s="14">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="R35" s="14">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="S35" s="14">
         <f t="shared" si="3"/>
@@ -2533,11 +2555,11 @@
       </c>
       <c r="T35" s="14">
         <f t="shared" si="3"/>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U35" s="15">
         <f>SUM(U4:U34)</f>
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="X35" s="24" t="s">
         <v>28</v>
@@ -2570,43 +2592,43 @@
       </c>
       <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>1809.3457943925234</v>
+        <v>1851.7543859649122</v>
       </c>
       <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>1592.2242990654206</v>
+        <v>1777.6842105263158</v>
       </c>
       <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>1447.4766355140187</v>
+        <v>1481.4035087719299</v>
       </c>
       <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>1954.0934579439252</v>
+        <v>2148.0350877192982</v>
       </c>
       <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>1519.8504672897197</v>
+        <v>1703.6140350877195</v>
       </c>
       <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>1592.2242990654206</v>
+        <v>1777.6842105263158</v>
       </c>
       <c r="Q36" s="4">
         <f>Q35*B38</f>
-        <v>578.99065420560748</v>
+        <v>740.70175438596493</v>
       </c>
       <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>1592.2242990654206</v>
+        <v>1777.6842105263158</v>
       </c>
       <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>1447.4766355140187</v>
+        <v>1481.4035087719299</v>
       </c>
       <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>1954.0934579439252</v>
+        <v>2148.0350877192982</v>
       </c>
       <c r="U36" s="8"/>
     </row>
@@ -2623,43 +2645,43 @@
       <c r="J37" s="4"/>
       <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>190.65420560747657</v>
+        <v>148.24561403508778</v>
       </c>
       <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>1316.7757009345794</v>
+        <v>1131.3157894736842</v>
       </c>
       <c r="M37" s="20">
         <f>B9-M36</f>
-        <v>-1447.4766355140187</v>
+        <v>-1481.4035087719299</v>
       </c>
       <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>-1954.0934579439252</v>
+        <v>-2148.0350877192982</v>
       </c>
       <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>1040.1495327102803</v>
+        <v>856.38596491228054</v>
       </c>
       <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>407.77570093457939</v>
+        <v>222.31578947368416</v>
       </c>
       <c r="Q37" s="17">
         <f>B8-Q36</f>
-        <v>1421.0093457943926</v>
+        <v>1259.2982456140351</v>
       </c>
       <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>30.77570093457939</v>
+        <v>-154.68421052631584</v>
       </c>
       <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>567.52336448598135</v>
+        <v>533.59649122807014</v>
       </c>
       <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>545.90654205607484</v>
+        <v>351.96491228070181</v>
       </c>
       <c r="U37" s="8"/>
     </row>
@@ -2669,7 +2691,7 @@
       </c>
       <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>72.373831775700936</v>
+        <v>74.070175438596493</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>

</xml_diff>

<commit_message>
updated for 17 tarikh
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>Meal list</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t xml:space="preserve">                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
   </si>
 </sst>
 </file>
@@ -702,7 +705,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -713,7 +716,7 @@
   <dimension ref="A1:AC104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -781,10 +784,12 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>2000</v>
+        <v>2638</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4">
+        <v>638</v>
+      </c>
       <c r="E3" s="32" t="s">
         <v>10</v>
       </c>
@@ -914,10 +919,12 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>2560</v>
+        <v>3142</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4">
+        <v>582</v>
+      </c>
       <c r="E5" s="6">
         <v>44471</v>
       </c>
@@ -983,9 +990,11 @@
         <v>11</v>
       </c>
       <c r="B6" s="4">
-        <v>1000</v>
-      </c>
-      <c r="C6" s="4"/>
+        <v>723</v>
+      </c>
+      <c r="C6" s="4">
+        <v>277</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="6">
         <v>44472</v>
@@ -1126,7 +1135,9 @@
         <v>2000</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4">
+        <v>717</v>
+      </c>
       <c r="E8" s="6">
         <v>44474</v>
       </c>
@@ -1191,8 +1202,12 @@
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="B9" s="4">
+        <v>557</v>
+      </c>
+      <c r="C9" s="4">
+        <v>543</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="6">
         <v>44475</v>
@@ -1469,15 +1484,15 @@
       </c>
       <c r="B13" s="10">
         <f>SUM(B3:B12)</f>
-        <v>18607</v>
+        <v>20107</v>
       </c>
       <c r="C13" s="26">
         <f>SUM(C3:C12)</f>
-        <v>1546</v>
+        <v>2366</v>
       </c>
       <c r="D13" s="26">
         <f>SUM(D3:D12)</f>
-        <v>409</v>
+        <v>2346</v>
       </c>
       <c r="E13" s="6">
         <v>44479</v>
@@ -1612,7 +1627,7 @@
       </c>
       <c r="D15" s="27">
         <f>C13-D13</f>
-        <v>1137</v>
+        <v>20</v>
       </c>
       <c r="E15" s="6">
         <v>44481</v>
@@ -1756,19 +1771,39 @@
       <c r="J17" s="6">
         <v>44483</v>
       </c>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>2</v>
+      </c>
+      <c r="M17" s="9">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>2</v>
+      </c>
+      <c r="O17" s="4">
+        <v>2</v>
+      </c>
+      <c r="P17" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>2</v>
+      </c>
+      <c r="R17" s="4">
+        <v>2</v>
+      </c>
+      <c r="S17" s="4">
+        <v>0</v>
+      </c>
+      <c r="T17" s="4">
+        <v>2</v>
+      </c>
       <c r="U17" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="X17" s="21">
         <v>44483</v>
@@ -1790,33 +1825,55 @@
       </c>
       <c r="B18" s="11">
         <f>B13-F35</f>
-        <v>924</v>
+        <v>1099</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="6">
         <v>44484</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="7">
+        <v>75</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="6">
         <v>44484</v>
       </c>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
+      <c r="K18" s="4">
+        <v>0</v>
+      </c>
+      <c r="L18" s="4">
+        <v>1</v>
+      </c>
+      <c r="M18" s="9">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4">
+        <v>1</v>
+      </c>
+      <c r="O18" s="4">
+        <v>2</v>
+      </c>
+      <c r="P18" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>2</v>
+      </c>
+      <c r="R18" s="4">
+        <v>2</v>
+      </c>
+      <c r="S18" s="4">
+        <v>0</v>
+      </c>
+      <c r="T18" s="4">
+        <v>2</v>
+      </c>
       <c r="U18" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X18" s="21">
         <v>44484</v>
@@ -1840,26 +1897,48 @@
       <c r="E19" s="6">
         <v>44485</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="7">
+        <v>1100</v>
+      </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="6">
         <v>44485</v>
       </c>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
+      <c r="K19" s="4">
+        <v>0</v>
+      </c>
+      <c r="L19" s="4">
+        <v>2</v>
+      </c>
+      <c r="M19" s="9">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4">
+        <v>2</v>
+      </c>
+      <c r="O19" s="4">
+        <v>1</v>
+      </c>
+      <c r="P19" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>2</v>
+      </c>
+      <c r="R19" s="4">
+        <v>2</v>
+      </c>
+      <c r="S19" s="4">
+        <v>1</v>
+      </c>
+      <c r="T19" s="4">
+        <v>2</v>
+      </c>
       <c r="U19" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="X19" s="21">
         <v>44485</v>
@@ -1883,26 +1962,48 @@
       <c r="E20" s="6">
         <v>44486</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="7">
+        <v>150</v>
+      </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="6">
         <v>44486</v>
       </c>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
+      <c r="K20" s="4">
+        <v>0</v>
+      </c>
+      <c r="L20" s="4">
+        <v>2</v>
+      </c>
+      <c r="M20" s="9">
+        <v>2</v>
+      </c>
+      <c r="N20" s="4">
+        <v>1</v>
+      </c>
+      <c r="O20" s="4">
+        <v>2</v>
+      </c>
+      <c r="P20" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>2</v>
+      </c>
+      <c r="R20" s="4">
+        <v>2</v>
+      </c>
+      <c r="S20" s="4">
+        <v>2</v>
+      </c>
+      <c r="T20" s="4">
+        <v>2</v>
+      </c>
       <c r="U20" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="X20" s="21">
         <v>44486</v>
@@ -2324,7 +2425,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="6">
@@ -2540,7 +2641,7 @@
       </c>
       <c r="F35" s="12">
         <f>SUM(F4:F34)</f>
-        <v>17683</v>
+        <v>19008</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -2554,43 +2655,43 @@
       </c>
       <c r="L35" s="14">
         <f>SUM(L4:L34)</f>
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="M35" s="14">
         <f t="shared" ref="M35:T35" si="3">SUM(M4:M34)</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N35" s="14">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="O35" s="14">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="Q35" s="14">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="R35" s="14">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="S35" s="14">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="T35" s="14">
         <f t="shared" si="3"/>
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="U35" s="15">
         <f>SUM(U4:U34)</f>
-        <v>241</v>
+        <v>298</v>
       </c>
       <c r="X35" s="24" t="s">
         <v>28</v>
@@ -2623,43 +2724,43 @@
       </c>
       <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>1834.3360995850624</v>
+        <v>1594.6308724832213</v>
       </c>
       <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>1907.7095435684648</v>
+        <v>2104.9127516778522</v>
       </c>
       <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>1467.4688796680498</v>
+        <v>1403.2751677852348</v>
       </c>
       <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>2201.2033195020749</v>
+        <v>2296.2684563758389</v>
       </c>
       <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>1834.3360995850624</v>
+        <v>2041.1275167785234</v>
       </c>
       <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>1907.7095435684648</v>
+        <v>2168.6979865771809</v>
       </c>
       <c r="Q36" s="4">
         <f>Q35*B38</f>
-        <v>880.48132780082994</v>
+        <v>1275.7046979865772</v>
       </c>
       <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>1907.7095435684648</v>
+        <v>2168.6979865771809</v>
       </c>
       <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>1467.4688796680498</v>
+        <v>1467.0604026845638</v>
       </c>
       <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>2274.5767634854774</v>
+        <v>2487.6241610738252</v>
       </c>
       <c r="U36" s="8"/>
     </row>
@@ -2676,43 +2777,43 @@
       <c r="J37" s="4"/>
       <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>165.66390041493764</v>
+        <v>1043.3691275167787</v>
       </c>
       <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>1001.2904564315352</v>
+        <v>804.08724832214784</v>
       </c>
       <c r="M37" s="20">
         <f>B9-M36</f>
-        <v>-1467.4688796680498</v>
+        <v>-846.27516778523477</v>
       </c>
       <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>-1201.2033195020749</v>
+        <v>-1573.2684563758389</v>
       </c>
       <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>725.66390041493764</v>
+        <v>1100.8724832214766</v>
       </c>
       <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>92.290456431535176</v>
+        <v>-168.69798657718093</v>
       </c>
       <c r="Q37" s="17">
         <f>B8-Q36</f>
-        <v>1119.5186721991699</v>
+        <v>724.29530201342277</v>
       </c>
       <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>-284.70954356846482</v>
+        <v>-545.69798657718093</v>
       </c>
       <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>547.53112033195021</v>
+        <v>547.93959731543623</v>
       </c>
       <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>225.42323651452261</v>
+        <v>12.375838926174765</v>
       </c>
       <c r="U37" s="8"/>
     </row>
@@ -2722,7 +2823,7 @@
       </c>
       <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>73.373443983402495</v>
+        <v>63.785234899328856</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>

</xml_diff>

<commit_message>
updated for 20 tarikh
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -715,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="F13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1061,7 +1061,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="4">
-        <v>2000</v>
+        <v>1900</v>
       </c>
       <c r="C7" s="4">
         <v>93</v>
@@ -1343,7 +1343,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="4">
-        <v>2015</v>
+        <v>2515</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1484,7 +1484,7 @@
       </c>
       <c r="B13" s="10">
         <f>SUM(B3:B12)</f>
-        <v>20107</v>
+        <v>20507</v>
       </c>
       <c r="C13" s="26">
         <f>SUM(C3:C12)</f>
@@ -1825,7 +1825,7 @@
       </c>
       <c r="B18" s="11">
         <f>B13-F35</f>
-        <v>1099</v>
+        <v>54</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2027,7 +2027,9 @@
       <c r="E21" s="6">
         <v>44487</v>
       </c>
-      <c r="F21" s="7"/>
+      <c r="F21" s="7">
+        <v>170</v>
+      </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4" t="s">
         <v>20</v>
@@ -2036,19 +2038,39 @@
       <c r="J21" s="6">
         <v>44487</v>
       </c>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
+      <c r="K21" s="4">
+        <v>0</v>
+      </c>
+      <c r="L21" s="4">
+        <v>2</v>
+      </c>
+      <c r="M21" s="9">
+        <v>2</v>
+      </c>
+      <c r="N21" s="4">
+        <v>2</v>
+      </c>
+      <c r="O21" s="4">
+        <v>2</v>
+      </c>
+      <c r="P21" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>2</v>
+      </c>
+      <c r="R21" s="4">
+        <v>2</v>
+      </c>
+      <c r="S21" s="4">
+        <v>2</v>
+      </c>
+      <c r="T21" s="4">
+        <v>2</v>
+      </c>
       <c r="U21" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="X21" s="21">
         <v>44487</v>
@@ -2072,26 +2094,48 @@
       <c r="E22" s="6">
         <v>44488</v>
       </c>
-      <c r="F22" s="7"/>
+      <c r="F22" s="7">
+        <v>170</v>
+      </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="6">
         <v>44488</v>
       </c>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
+      <c r="K22" s="4">
+        <v>0</v>
+      </c>
+      <c r="L22" s="4">
+        <v>1</v>
+      </c>
+      <c r="M22" s="9">
+        <v>2</v>
+      </c>
+      <c r="N22" s="4">
+        <v>2</v>
+      </c>
+      <c r="O22" s="4">
+        <v>2</v>
+      </c>
+      <c r="P22" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>3</v>
+      </c>
+      <c r="R22" s="4">
+        <v>2</v>
+      </c>
+      <c r="S22" s="4">
+        <v>2</v>
+      </c>
+      <c r="T22" s="4">
+        <v>2</v>
+      </c>
       <c r="U22" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="X22" s="21">
         <v>44488</v>
@@ -2115,26 +2159,48 @@
       <c r="E23" s="6">
         <v>44489</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="F23" s="7">
+        <v>1105</v>
+      </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="6">
         <v>44489</v>
       </c>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
+      <c r="K23" s="4">
+        <v>2</v>
+      </c>
+      <c r="L23" s="4">
+        <v>2</v>
+      </c>
+      <c r="M23" s="9">
+        <v>2</v>
+      </c>
+      <c r="N23" s="4">
+        <v>2</v>
+      </c>
+      <c r="O23" s="4">
+        <v>2</v>
+      </c>
+      <c r="P23" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>4</v>
+      </c>
+      <c r="R23" s="4">
+        <v>2</v>
+      </c>
+      <c r="S23" s="4">
+        <v>2</v>
+      </c>
+      <c r="T23" s="4">
+        <v>2</v>
+      </c>
       <c r="U23" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="X23" s="21">
         <v>44489</v>
@@ -2641,7 +2707,7 @@
       </c>
       <c r="F35" s="12">
         <f>SUM(F4:F34)</f>
-        <v>19008</v>
+        <v>20453</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -2651,47 +2717,47 @@
       </c>
       <c r="K35" s="14">
         <f>SUM(K4:K34)</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L35" s="14">
         <f>SUM(L4:L34)</f>
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="M35" s="14">
         <f t="shared" ref="M35:T35" si="3">SUM(M4:M34)</f>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="N35" s="14">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="O35" s="14">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="Q35" s="14">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="R35" s="14">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="S35" s="14">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="T35" s="14">
         <f t="shared" si="3"/>
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="U35" s="15">
         <f>SUM(U4:U34)</f>
-        <v>298</v>
+        <v>356</v>
       </c>
       <c r="X35" s="24" t="s">
         <v>28</v>
@@ -2724,43 +2790,43 @@
       </c>
       <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>1594.6308724832213</v>
+        <v>1551.2106741573034</v>
       </c>
       <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>2104.9127516778522</v>
+        <v>2183.1853932584272</v>
       </c>
       <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>1403.2751677852348</v>
+        <v>1608.6629213483147</v>
       </c>
       <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>2296.2684563758389</v>
+        <v>2412.9943820224721</v>
       </c>
       <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>2041.1275167785234</v>
+        <v>2183.1853932584272</v>
       </c>
       <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>2168.6979865771809</v>
+        <v>2298.0898876404494</v>
       </c>
       <c r="Q36" s="4">
         <f>Q35*B38</f>
-        <v>1275.7046979865772</v>
+        <v>1666.1151685393259</v>
       </c>
       <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>2168.6979865771809</v>
+        <v>2298.0898876404494</v>
       </c>
       <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>1467.0604026845638</v>
+        <v>1666.1151685393259</v>
       </c>
       <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>2487.6241610738252</v>
+        <v>2585.3511235955057</v>
       </c>
       <c r="U36" s="8"/>
     </row>
@@ -2777,43 +2843,43 @@
       <c r="J37" s="4"/>
       <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>1043.3691275167787</v>
+        <v>1086.7893258426966</v>
       </c>
       <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>804.08724832214784</v>
+        <v>725.81460674157279</v>
       </c>
       <c r="M37" s="20">
         <f>B9-M36</f>
-        <v>-846.27516778523477</v>
+        <v>-1051.6629213483147</v>
       </c>
       <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>-1573.2684563758389</v>
+        <v>-1689.9943820224721</v>
       </c>
       <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>1100.8724832214766</v>
+        <v>958.81460674157279</v>
       </c>
       <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>-168.69798657718093</v>
+        <v>-398.08988764044943</v>
       </c>
       <c r="Q37" s="17">
         <f>B8-Q36</f>
-        <v>724.29530201342277</v>
+        <v>333.88483146067415</v>
       </c>
       <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>-545.69798657718093</v>
+        <v>-675.08988764044943</v>
       </c>
       <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>547.93959731543623</v>
+        <v>848.88483146067415</v>
       </c>
       <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>12.375838926174765</v>
+        <v>-85.351123595505669</v>
       </c>
       <c r="U37" s="8"/>
     </row>
@@ -2823,7 +2889,7 @@
       </c>
       <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>63.785234899328856</v>
+        <v>57.452247191011239</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>

</xml_diff>

<commit_message>
updated for 22 tarikh
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>Meal list</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>225 taka baki</t>
   </si>
 </sst>
 </file>
@@ -715,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -727,6 +730,7 @@
     <col min="4" max="4" width="40.28515625" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
     <col min="20" max="20" width="12.28515625" customWidth="1"/>
     <col min="21" max="21" width="14.42578125" customWidth="1"/>
@@ -784,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>2638</v>
+        <v>3188</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4">
@@ -1203,7 +1207,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="4">
-        <v>557</v>
+        <v>1557</v>
       </c>
       <c r="C9" s="4">
         <v>543</v>
@@ -1484,7 +1488,7 @@
       </c>
       <c r="B13" s="10">
         <f>SUM(B3:B12)</f>
-        <v>20507</v>
+        <v>22057</v>
       </c>
       <c r="C13" s="26">
         <f>SUM(C3:C12)</f>
@@ -1825,7 +1829,7 @@
       </c>
       <c r="B18" s="11">
         <f>B13-F35</f>
-        <v>54</v>
+        <v>-871</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2160,7 +2164,7 @@
         <v>44489</v>
       </c>
       <c r="F23" s="7">
-        <v>1105</v>
+        <v>1205</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -2226,26 +2230,50 @@
       <c r="E24" s="6">
         <v>44490</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="4"/>
+      <c r="F24" s="7">
+        <v>2375</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="6">
         <v>44490</v>
       </c>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
+      <c r="K24" s="4">
+        <v>2</v>
+      </c>
+      <c r="L24" s="4">
+        <v>2</v>
+      </c>
+      <c r="M24" s="9">
+        <v>2</v>
+      </c>
+      <c r="N24" s="4">
+        <v>2</v>
+      </c>
+      <c r="O24" s="4">
+        <v>2</v>
+      </c>
+      <c r="P24" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>2</v>
+      </c>
+      <c r="R24" s="4">
+        <v>2</v>
+      </c>
+      <c r="S24" s="4">
+        <v>2</v>
+      </c>
+      <c r="T24" s="4">
+        <v>2</v>
+      </c>
       <c r="U24" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="X24" s="21">
         <v>44490</v>
@@ -2707,7 +2735,7 @@
       </c>
       <c r="F35" s="12">
         <f>SUM(F4:F34)</f>
-        <v>20453</v>
+        <v>22928</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -2717,47 +2745,47 @@
       </c>
       <c r="K35" s="14">
         <f>SUM(K4:K34)</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L35" s="14">
         <f>SUM(L4:L34)</f>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M35" s="14">
         <f t="shared" ref="M35:T35" si="3">SUM(M4:M34)</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N35" s="14">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O35" s="14">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="Q35" s="14">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="R35" s="14">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="S35" s="14">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="T35" s="14">
         <f t="shared" si="3"/>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="U35" s="15">
         <f>SUM(U4:U34)</f>
-        <v>356</v>
+        <v>376</v>
       </c>
       <c r="X35" s="24" t="s">
         <v>28</v>
@@ -2790,43 +2818,43 @@
       </c>
       <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>1551.2106741573034</v>
+        <v>1768.3829787234042</v>
       </c>
       <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>2183.1853932584272</v>
+        <v>2439.1489361702129</v>
       </c>
       <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>1608.6629213483147</v>
+        <v>1829.3617021276596</v>
       </c>
       <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>2412.9943820224721</v>
+        <v>2683.0638297872342</v>
       </c>
       <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>2183.1853932584272</v>
+        <v>2439.1489361702129</v>
       </c>
       <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>2298.0898876404494</v>
+        <v>2561.1063829787236</v>
       </c>
       <c r="Q36" s="4">
         <f>Q35*B38</f>
-        <v>1666.1151685393259</v>
+        <v>1890.3404255319149</v>
       </c>
       <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>2298.0898876404494</v>
+        <v>2561.1063829787236</v>
       </c>
       <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>1666.1151685393259</v>
+        <v>1890.3404255319149</v>
       </c>
       <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>2585.3511235955057</v>
+        <v>2866</v>
       </c>
       <c r="U36" s="8"/>
     </row>
@@ -2843,43 +2871,43 @@
       <c r="J37" s="4"/>
       <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>1086.7893258426966</v>
+        <v>1419.6170212765958</v>
       </c>
       <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>725.81460674157279</v>
+        <v>469.85106382978711</v>
       </c>
       <c r="M37" s="20">
         <f>B9-M36</f>
-        <v>-1051.6629213483147</v>
+        <v>-272.36170212765956</v>
       </c>
       <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>-1689.9943820224721</v>
+        <v>-1960.0638297872342</v>
       </c>
       <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>958.81460674157279</v>
+        <v>702.85106382978711</v>
       </c>
       <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>-398.08988764044943</v>
+        <v>-661.10638297872356</v>
       </c>
       <c r="Q37" s="17">
         <f>B8-Q36</f>
-        <v>333.88483146067415</v>
+        <v>109.65957446808511</v>
       </c>
       <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>-675.08988764044943</v>
+        <v>-938.10638297872356</v>
       </c>
       <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>848.88483146067415</v>
+        <v>624.65957446808511</v>
       </c>
       <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>-85.351123595505669</v>
+        <v>-366</v>
       </c>
       <c r="U37" s="8"/>
     </row>
@@ -2889,7 +2917,7 @@
       </c>
       <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>57.452247191011239</v>
+        <v>60.978723404255319</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>

</xml_diff>

<commit_message>
updated for 24 tarikh
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -708,7 +708,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -994,7 +994,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="4">
-        <v>723</v>
+        <v>1718</v>
       </c>
       <c r="C6" s="4">
         <v>277</v>
@@ -1136,7 +1136,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4">
@@ -1278,7 +1278,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="4">
-        <v>1623</v>
+        <v>2183</v>
       </c>
       <c r="C10" s="4">
         <v>977</v>
@@ -1488,7 +1488,7 @@
       </c>
       <c r="B13" s="10">
         <f>SUM(B3:B12)</f>
-        <v>22057</v>
+        <v>24112</v>
       </c>
       <c r="C13" s="26">
         <f>SUM(C3:C12)</f>
@@ -1829,7 +1829,7 @@
       </c>
       <c r="B18" s="11">
         <f>B13-F35</f>
-        <v>-871</v>
+        <v>784</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2164,7 +2164,7 @@
         <v>44489</v>
       </c>
       <c r="F23" s="7">
-        <v>1205</v>
+        <v>1305</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -2299,26 +2299,48 @@
       <c r="E25" s="6">
         <v>44491</v>
       </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="7">
+        <v>115</v>
+      </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="6">
         <v>44491</v>
       </c>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
+      <c r="K25" s="4">
+        <v>2</v>
+      </c>
+      <c r="L25" s="4">
+        <v>2</v>
+      </c>
+      <c r="M25" s="9">
+        <v>2</v>
+      </c>
+      <c r="N25" s="4">
+        <v>2</v>
+      </c>
+      <c r="O25" s="4">
+        <v>2</v>
+      </c>
+      <c r="P25" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>2</v>
+      </c>
+      <c r="R25" s="4">
+        <v>2</v>
+      </c>
+      <c r="S25" s="4">
+        <v>2</v>
+      </c>
+      <c r="T25" s="4">
+        <v>2</v>
+      </c>
       <c r="U25" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="X25" s="21">
         <v>44491</v>
@@ -2351,19 +2373,39 @@
       <c r="J26" s="6">
         <v>44492</v>
       </c>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
+      <c r="K26" s="4">
+        <v>1</v>
+      </c>
+      <c r="L26" s="4">
+        <v>0</v>
+      </c>
+      <c r="M26" s="9">
+        <v>2</v>
+      </c>
+      <c r="N26" s="4">
+        <v>0</v>
+      </c>
+      <c r="O26" s="4">
+        <v>2</v>
+      </c>
+      <c r="P26" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>2</v>
+      </c>
+      <c r="R26" s="4">
+        <v>2</v>
+      </c>
+      <c r="S26" s="4">
+        <v>2</v>
+      </c>
+      <c r="T26" s="4">
+        <v>2</v>
+      </c>
       <c r="U26" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="X26" s="21">
         <v>44492</v>
@@ -2387,26 +2429,48 @@
       <c r="E27" s="6">
         <v>44493</v>
       </c>
-      <c r="F27" s="7"/>
+      <c r="F27" s="7">
+        <v>185</v>
+      </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="6">
         <v>44493</v>
       </c>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
+      <c r="K27" s="4">
+        <v>2</v>
+      </c>
+      <c r="L27" s="4">
+        <v>0</v>
+      </c>
+      <c r="M27" s="9">
+        <v>2</v>
+      </c>
+      <c r="N27" s="4">
+        <v>0</v>
+      </c>
+      <c r="O27" s="4">
+        <v>2</v>
+      </c>
+      <c r="P27" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>2</v>
+      </c>
+      <c r="R27" s="4">
+        <v>2</v>
+      </c>
+      <c r="S27" s="4">
+        <v>2</v>
+      </c>
+      <c r="T27" s="4">
+        <v>2</v>
+      </c>
       <c r="U27" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X27" s="21">
         <v>44493</v>
@@ -2735,7 +2799,7 @@
       </c>
       <c r="F35" s="12">
         <f>SUM(F4:F34)</f>
-        <v>22928</v>
+        <v>23328</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -2745,47 +2809,47 @@
       </c>
       <c r="K35" s="14">
         <f>SUM(K4:K34)</f>
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="L35" s="14">
         <f>SUM(L4:L34)</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="M35" s="14">
         <f t="shared" ref="M35:T35" si="3">SUM(M4:M34)</f>
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N35" s="14">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O35" s="14">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="Q35" s="14">
         <f t="shared" si="3"/>
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="R35" s="14">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="S35" s="14">
         <f t="shared" si="3"/>
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="T35" s="14">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="U35" s="15">
         <f>SUM(U4:U34)</f>
-        <v>376</v>
+        <v>425</v>
       </c>
       <c r="X35" s="24" t="s">
         <v>28</v>
@@ -2818,43 +2882,43 @@
       </c>
       <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>1768.3829787234042</v>
+        <v>1866.24</v>
       </c>
       <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>2439.1489361702129</v>
+        <v>2305.3552941176472</v>
       </c>
       <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>1829.3617021276596</v>
+        <v>1976.0188235294117</v>
       </c>
       <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>2683.0638297872342</v>
+        <v>2524.9129411764707</v>
       </c>
       <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>2439.1489361702129</v>
+        <v>2524.9129411764707</v>
       </c>
       <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>2561.1063829787236</v>
+        <v>2524.9129411764707</v>
       </c>
       <c r="Q36" s="4">
         <f>Q35*B38</f>
-        <v>1890.3404255319149</v>
+        <v>2030.9082352941177</v>
       </c>
       <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>2561.1063829787236</v>
+        <v>2634.6917647058826</v>
       </c>
       <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>1890.3404255319149</v>
+        <v>2030.9082352941177</v>
       </c>
       <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>2866</v>
+        <v>2909.1388235294116</v>
       </c>
       <c r="U36" s="8"/>
     </row>
@@ -2871,43 +2935,43 @@
       <c r="J37" s="4"/>
       <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>1419.6170212765958</v>
+        <v>1321.76</v>
       </c>
       <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>469.85106382978711</v>
+        <v>603.64470588235281</v>
       </c>
       <c r="M37" s="20">
         <f>B9-M36</f>
-        <v>-272.36170212765956</v>
+        <v>-419.01882352941175</v>
       </c>
       <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>-1960.0638297872342</v>
+        <v>-806.91294117647067</v>
       </c>
       <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>702.85106382978711</v>
+        <v>617.08705882352933</v>
       </c>
       <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>-661.10638297872356</v>
+        <v>-624.91294117647067</v>
       </c>
       <c r="Q37" s="17">
         <f>B8-Q36</f>
-        <v>109.65957446808511</v>
+        <v>469.09176470588227</v>
       </c>
       <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>-938.10638297872356</v>
+        <v>-451.69176470588263</v>
       </c>
       <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>624.65957446808511</v>
+        <v>484.09176470588227</v>
       </c>
       <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>-366</v>
+        <v>-409.13882352941164</v>
       </c>
       <c r="U37" s="8"/>
     </row>
@@ -2917,7 +2981,7 @@
       </c>
       <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>60.978723404255319</v>
+        <v>54.889411764705883</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>

</xml_diff>

<commit_message>
updated for 25 tarikh
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -134,7 +134,7 @@
     <t xml:space="preserve">    </t>
   </si>
   <si>
-    <t>225 taka baki</t>
+    <t>275 taka baki</t>
   </si>
 </sst>
 </file>
@@ -708,7 +708,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -788,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>3188</v>
+        <v>3268</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4">
@@ -1426,7 +1426,7 @@
         <v>44478</v>
       </c>
       <c r="F12" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -1488,7 +1488,7 @@
       </c>
       <c r="B13" s="10">
         <f>SUM(B3:B12)</f>
-        <v>24112</v>
+        <v>24192</v>
       </c>
       <c r="C13" s="26">
         <f>SUM(C3:C12)</f>
@@ -1829,7 +1829,7 @@
       </c>
       <c r="B18" s="11">
         <f>B13-F35</f>
-        <v>784</v>
+        <v>454</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1837,7 +1837,7 @@
         <v>44484</v>
       </c>
       <c r="F18" s="7">
-        <v>75</v>
+        <v>175</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -2494,26 +2494,46 @@
       <c r="E28" s="6">
         <v>44494</v>
       </c>
-      <c r="F28" s="7"/>
+      <c r="F28" s="7">
+        <v>160</v>
+      </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="6">
         <v>44494</v>
       </c>
-      <c r="K28" s="4"/>
+      <c r="K28" s="4">
+        <v>2</v>
+      </c>
       <c r="L28" s="4"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
+      <c r="M28" s="9">
+        <v>2</v>
+      </c>
+      <c r="N28" s="4">
+        <v>0</v>
+      </c>
+      <c r="O28" s="4">
+        <v>2</v>
+      </c>
+      <c r="P28" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>2</v>
+      </c>
+      <c r="R28" s="4">
+        <v>2</v>
+      </c>
+      <c r="S28" s="4">
+        <v>2</v>
+      </c>
+      <c r="T28" s="4">
+        <v>2</v>
+      </c>
       <c r="U28" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X28" s="21">
         <v>44494</v>
@@ -2799,7 +2819,7 @@
       </c>
       <c r="F35" s="12">
         <f>SUM(F4:F34)</f>
-        <v>23328</v>
+        <v>23738</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -2809,7 +2829,7 @@
       </c>
       <c r="K35" s="14">
         <f>SUM(K4:K34)</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L35" s="14">
         <f>SUM(L4:L34)</f>
@@ -2817,7 +2837,7 @@
       </c>
       <c r="M35" s="14">
         <f t="shared" ref="M35:T35" si="3">SUM(M4:M34)</f>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N35" s="14">
         <f t="shared" si="3"/>
@@ -2825,31 +2845,31 @@
       </c>
       <c r="O35" s="14">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q35" s="14">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="R35" s="14">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S35" s="14">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="T35" s="14">
         <f t="shared" si="3"/>
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="U35" s="15">
         <f>SUM(U4:U34)</f>
-        <v>425</v>
+        <v>441</v>
       </c>
       <c r="X35" s="24" t="s">
         <v>28</v>
@@ -2882,43 +2902,43 @@
       </c>
       <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>1866.24</v>
+        <v>1937.7959183673468</v>
       </c>
       <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>2305.3552941176472</v>
+        <v>2260.7619047619046</v>
       </c>
       <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>1976.0188235294117</v>
+        <v>2045.4512471655328</v>
       </c>
       <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>2524.9129411764707</v>
+        <v>2476.0725623582766</v>
       </c>
       <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>2524.9129411764707</v>
+        <v>2583.7278911564626</v>
       </c>
       <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>2524.9129411764707</v>
+        <v>2583.7278911564626</v>
       </c>
       <c r="Q36" s="4">
         <f>Q35*B38</f>
-        <v>2030.9082352941177</v>
+        <v>2099.2789115646256</v>
       </c>
       <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>2634.6917647058826</v>
+        <v>2691.3832199546482</v>
       </c>
       <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>2030.9082352941177</v>
+        <v>2099.2789115646256</v>
       </c>
       <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>2909.1388235294116</v>
+        <v>2960.5215419501133</v>
       </c>
       <c r="U36" s="8"/>
     </row>
@@ -2935,43 +2955,43 @@
       <c r="J37" s="4"/>
       <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>1321.76</v>
+        <v>1330.2040816326532</v>
       </c>
       <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>603.64470588235281</v>
+        <v>648.23809523809541</v>
       </c>
       <c r="M37" s="20">
         <f>B9-M36</f>
-        <v>-419.01882352941175</v>
+        <v>-488.45124716553278</v>
       </c>
       <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>-806.91294117647067</v>
+        <v>-758.07256235827663</v>
       </c>
       <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>617.08705882352933</v>
+        <v>558.27210884353735</v>
       </c>
       <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>-624.91294117647067</v>
+        <v>-683.72789115646265</v>
       </c>
       <c r="Q37" s="17">
         <f>B8-Q36</f>
-        <v>469.09176470588227</v>
+        <v>400.72108843537444</v>
       </c>
       <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>-451.69176470588263</v>
+        <v>-508.38321995464821</v>
       </c>
       <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>484.09176470588227</v>
+        <v>415.72108843537444</v>
       </c>
       <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>-409.13882352941164</v>
+        <v>-460.52154195011326</v>
       </c>
       <c r="U37" s="8"/>
     </row>
@@ -2981,7 +3001,7 @@
       </c>
       <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>54.889411764705883</v>
+        <v>53.827664399092967</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>

</xml_diff>

<commit_message>
updated for 26 tarikh
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -719,7 +719,7 @@
   <dimension ref="A1:AC104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1829,7 +1829,7 @@
       </c>
       <c r="B18" s="11">
         <f>B13-F35</f>
-        <v>454</v>
+        <v>-486</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2506,7 +2506,9 @@
       <c r="K28" s="4">
         <v>2</v>
       </c>
-      <c r="L28" s="4"/>
+      <c r="L28" s="4">
+        <v>0</v>
+      </c>
       <c r="M28" s="9">
         <v>2</v>
       </c>
@@ -2557,26 +2559,48 @@
       <c r="E29" s="6">
         <v>44495</v>
       </c>
-      <c r="F29" s="7"/>
+      <c r="F29" s="7">
+        <v>940</v>
+      </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="6">
         <v>44495</v>
       </c>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
+      <c r="K29" s="4">
+        <v>2</v>
+      </c>
+      <c r="L29" s="4">
+        <v>0</v>
+      </c>
+      <c r="M29" s="9">
+        <v>2</v>
+      </c>
+      <c r="N29" s="4">
+        <v>0</v>
+      </c>
+      <c r="O29" s="4">
+        <v>2</v>
+      </c>
+      <c r="P29" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q29" s="4">
+        <v>2</v>
+      </c>
+      <c r="R29" s="4">
+        <v>2</v>
+      </c>
+      <c r="S29" s="4">
+        <v>2</v>
+      </c>
+      <c r="T29" s="4">
+        <v>2</v>
+      </c>
       <c r="U29" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X29" s="21">
         <v>44495</v>
@@ -2819,7 +2843,7 @@
       </c>
       <c r="F35" s="12">
         <f>SUM(F4:F34)</f>
-        <v>23738</v>
+        <v>24678</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -2829,7 +2853,7 @@
       </c>
       <c r="K35" s="14">
         <f>SUM(K4:K34)</f>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L35" s="14">
         <f>SUM(L4:L34)</f>
@@ -2837,7 +2861,7 @@
       </c>
       <c r="M35" s="14">
         <f t="shared" ref="M35:T35" si="3">SUM(M4:M34)</f>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="N35" s="14">
         <f t="shared" si="3"/>
@@ -2845,31 +2869,31 @@
       </c>
       <c r="O35" s="14">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="Q35" s="14">
         <f t="shared" si="3"/>
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R35" s="14">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="S35" s="14">
         <f t="shared" si="3"/>
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="T35" s="14">
         <f t="shared" si="3"/>
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="U35" s="15">
         <f>SUM(U4:U34)</f>
-        <v>441</v>
+        <v>457</v>
       </c>
       <c r="X35" s="24" t="s">
         <v>28</v>
@@ -2902,43 +2926,43 @@
       </c>
       <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>1937.7959183673468</v>
+        <v>2052</v>
       </c>
       <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>2260.7619047619046</v>
+        <v>2268</v>
       </c>
       <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>2045.4512471655328</v>
+        <v>2160</v>
       </c>
       <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>2476.0725623582766</v>
+        <v>2484</v>
       </c>
       <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>2583.7278911564626</v>
+        <v>2700</v>
       </c>
       <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>2583.7278911564626</v>
+        <v>2700</v>
       </c>
       <c r="Q36" s="4">
         <f>Q35*B38</f>
-        <v>2099.2789115646256</v>
+        <v>2214</v>
       </c>
       <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>2691.3832199546482</v>
+        <v>2808</v>
       </c>
       <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>2099.2789115646256</v>
+        <v>2214</v>
       </c>
       <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>2960.5215419501133</v>
+        <v>3078</v>
       </c>
       <c r="U36" s="8"/>
     </row>
@@ -2955,43 +2979,43 @@
       <c r="J37" s="4"/>
       <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>1330.2040816326532</v>
+        <v>1216</v>
       </c>
       <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>648.23809523809541</v>
+        <v>641</v>
       </c>
       <c r="M37" s="20">
         <f>B9-M36</f>
-        <v>-488.45124716553278</v>
+        <v>-603</v>
       </c>
       <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>-758.07256235827663</v>
+        <v>-766</v>
       </c>
       <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>558.27210884353735</v>
+        <v>442</v>
       </c>
       <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>-683.72789115646265</v>
+        <v>-800</v>
       </c>
       <c r="Q37" s="17">
         <f>B8-Q36</f>
-        <v>400.72108843537444</v>
+        <v>286</v>
       </c>
       <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>-508.38321995464821</v>
+        <v>-625</v>
       </c>
       <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>415.72108843537444</v>
+        <v>301</v>
       </c>
       <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>-460.52154195011326</v>
+        <v>-578</v>
       </c>
       <c r="U37" s="8"/>
     </row>
@@ -3001,7 +3025,7 @@
       </c>
       <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>53.827664399092967</v>
+        <v>54</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>

</xml_diff>

<commit_message>
updated for 27 tarikh
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -708,7 +708,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="H19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1065,7 +1065,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="4">
-        <v>1900</v>
+        <v>2500</v>
       </c>
       <c r="C7" s="4">
         <v>93</v>
@@ -1488,7 +1488,7 @@
       </c>
       <c r="B13" s="10">
         <f>SUM(B3:B12)</f>
-        <v>24192</v>
+        <v>24792</v>
       </c>
       <c r="C13" s="26">
         <f>SUM(C3:C12)</f>
@@ -1829,7 +1829,7 @@
       </c>
       <c r="B18" s="11">
         <f>B13-F35</f>
-        <v>-486</v>
+        <v>114</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2522,7 +2522,7 @@
         <v>2</v>
       </c>
       <c r="Q28" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R28" s="4">
         <v>2</v>
@@ -2535,7 +2535,7 @@
       </c>
       <c r="U28" s="8">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="X28" s="21">
         <v>44494</v>
@@ -2587,7 +2587,7 @@
         <v>2</v>
       </c>
       <c r="Q29" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R29" s="4">
         <v>2</v>
@@ -2600,7 +2600,7 @@
       </c>
       <c r="U29" s="8">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="X29" s="21">
         <v>44495</v>
@@ -2633,19 +2633,39 @@
       <c r="J30" s="6">
         <v>44496</v>
       </c>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-      <c r="T30" s="4"/>
+      <c r="K30" s="4">
+        <v>2</v>
+      </c>
+      <c r="L30" s="4">
+        <v>0</v>
+      </c>
+      <c r="M30" s="9">
+        <v>2</v>
+      </c>
+      <c r="N30" s="4">
+        <v>0</v>
+      </c>
+      <c r="O30" s="4">
+        <v>2</v>
+      </c>
+      <c r="P30" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>0</v>
+      </c>
+      <c r="R30" s="4">
+        <v>2</v>
+      </c>
+      <c r="S30" s="4">
+        <v>2</v>
+      </c>
+      <c r="T30" s="4">
+        <v>2</v>
+      </c>
       <c r="U30" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="X30" s="21">
         <v>44496</v>
@@ -2853,7 +2873,7 @@
       </c>
       <c r="K35" s="14">
         <f>SUM(K4:K34)</f>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="L35" s="14">
         <f>SUM(L4:L34)</f>
@@ -2861,7 +2881,7 @@
       </c>
       <c r="M35" s="14">
         <f t="shared" ref="M35:T35" si="3">SUM(M4:M34)</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N35" s="14">
         <f t="shared" si="3"/>
@@ -2869,31 +2889,31 @@
       </c>
       <c r="O35" s="14">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q35" s="14">
         <f t="shared" si="3"/>
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="R35" s="14">
         <f t="shared" si="3"/>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="S35" s="14">
         <f t="shared" si="3"/>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T35" s="14">
         <f t="shared" si="3"/>
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="U35" s="15">
         <f>SUM(U4:U34)</f>
-        <v>457</v>
+        <v>467</v>
       </c>
       <c r="X35" s="24" t="s">
         <v>28</v>
@@ -2926,43 +2946,43 @@
       </c>
       <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>2052</v>
+        <v>2113.7473233404712</v>
       </c>
       <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>2268</v>
+        <v>2219.4346895074946</v>
       </c>
       <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>2160</v>
+        <v>2219.4346895074946</v>
       </c>
       <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>2484</v>
+        <v>2430.8094218415417</v>
       </c>
       <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>2700</v>
+        <v>2747.8715203426123</v>
       </c>
       <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>2700</v>
+        <v>2747.8715203426123</v>
       </c>
       <c r="Q36" s="4">
         <f>Q35*B38</f>
-        <v>2214</v>
+        <v>1955.2162740899357</v>
       </c>
       <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>2808</v>
+        <v>2853.5588865096361</v>
       </c>
       <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>2214</v>
+        <v>2272.2783725910062</v>
       </c>
       <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>3078</v>
+        <v>3117.7773019271949</v>
       </c>
       <c r="U36" s="8"/>
     </row>
@@ -2979,43 +2999,43 @@
       <c r="J37" s="4"/>
       <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>1216</v>
+        <v>1154.2526766595288</v>
       </c>
       <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>641</v>
+        <v>689.56531049250543</v>
       </c>
       <c r="M37" s="20">
         <f>B9-M36</f>
-        <v>-603</v>
+        <v>-662.43468950749457</v>
       </c>
       <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>-766</v>
+        <v>-712.80942184154173</v>
       </c>
       <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>442</v>
+        <v>394.12847965738774</v>
       </c>
       <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>-800</v>
+        <v>-247.87152034261226</v>
       </c>
       <c r="Q37" s="17">
         <f>B8-Q36</f>
-        <v>286</v>
+        <v>544.78372591006428</v>
       </c>
       <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>-625</v>
+        <v>-670.55888650963607</v>
       </c>
       <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>301</v>
+        <v>242.72162740899375</v>
       </c>
       <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>-578</v>
+        <v>-617.77730192719491</v>
       </c>
       <c r="U37" s="8"/>
     </row>
@@ -3025,7 +3045,7 @@
       </c>
       <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>54</v>
+        <v>52.843683083511777</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>

</xml_diff>

<commit_message>
updated for 29 tarikh
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -788,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>3268</v>
+        <v>4888</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4">
@@ -923,7 +923,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>3142</v>
+        <v>3292</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="B13" s="10">
         <f>SUM(B3:B12)</f>
-        <v>24792</v>
+        <v>26562</v>
       </c>
       <c r="C13" s="26">
         <f>SUM(C3:C12)</f>
@@ -1829,7 +1829,7 @@
       </c>
       <c r="B18" s="11">
         <f>B13-F35</f>
-        <v>114</v>
+        <v>54</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2624,7 +2624,9 @@
       <c r="E30" s="6">
         <v>44496</v>
       </c>
-      <c r="F30" s="7"/>
+      <c r="F30" s="7">
+        <v>1620</v>
+      </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4" t="s">
         <v>35</v>
@@ -2689,26 +2691,48 @@
       <c r="E31" s="6">
         <v>44497</v>
       </c>
-      <c r="F31" s="7"/>
+      <c r="F31" s="7">
+        <v>210</v>
+      </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="6">
         <v>44497</v>
       </c>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
+      <c r="K31" s="4">
+        <v>2</v>
+      </c>
+      <c r="L31" s="4">
+        <v>0</v>
+      </c>
+      <c r="M31" s="9">
+        <v>1</v>
+      </c>
+      <c r="N31" s="4">
+        <v>0</v>
+      </c>
+      <c r="O31" s="4">
+        <v>2</v>
+      </c>
+      <c r="P31" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>0</v>
+      </c>
+      <c r="R31" s="4">
+        <v>2</v>
+      </c>
+      <c r="S31" s="4">
+        <v>2</v>
+      </c>
+      <c r="T31" s="4">
+        <v>2</v>
+      </c>
       <c r="U31" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="X31" s="21">
         <v>44497</v>
@@ -2739,19 +2763,39 @@
       <c r="J32" s="6">
         <v>44498</v>
       </c>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
+      <c r="K32" s="4">
+        <v>2</v>
+      </c>
+      <c r="L32" s="4">
+        <v>0</v>
+      </c>
+      <c r="M32" s="9">
+        <v>0</v>
+      </c>
+      <c r="N32" s="4">
+        <v>0</v>
+      </c>
+      <c r="O32" s="4">
+        <v>2</v>
+      </c>
+      <c r="P32" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>0</v>
+      </c>
+      <c r="R32" s="4">
+        <v>2</v>
+      </c>
+      <c r="S32" s="4">
+        <v>2</v>
+      </c>
+      <c r="T32" s="4">
+        <v>2</v>
+      </c>
       <c r="U32" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X32" s="21">
         <v>44498</v>
@@ -2863,7 +2907,7 @@
       </c>
       <c r="F35" s="12">
         <f>SUM(F4:F34)</f>
-        <v>24678</v>
+        <v>26508</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -2873,7 +2917,7 @@
       </c>
       <c r="K35" s="14">
         <f>SUM(K4:K34)</f>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L35" s="14">
         <f>SUM(L4:L34)</f>
@@ -2881,7 +2925,7 @@
       </c>
       <c r="M35" s="14">
         <f t="shared" ref="M35:T35" si="3">SUM(M4:M34)</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N35" s="14">
         <f t="shared" si="3"/>
@@ -2889,11 +2933,11 @@
       </c>
       <c r="O35" s="14">
         <f t="shared" si="3"/>
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="3"/>
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="Q35" s="14">
         <f t="shared" si="3"/>
@@ -2901,19 +2945,19 @@
       </c>
       <c r="R35" s="14">
         <f t="shared" si="3"/>
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="S35" s="14">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="T35" s="14">
         <f t="shared" si="3"/>
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="U35" s="15">
         <f>SUM(U4:U34)</f>
-        <v>467</v>
+        <v>492</v>
       </c>
       <c r="X35" s="24" t="s">
         <v>28</v>
@@ -2946,43 +2990,43 @@
       </c>
       <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>2113.7473233404712</v>
+        <v>2370.6341463414633</v>
       </c>
       <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>2219.4346895074946</v>
+        <v>2262.8780487804879</v>
       </c>
       <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>2219.4346895074946</v>
+        <v>2316.7560975609754</v>
       </c>
       <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>2430.8094218415417</v>
+        <v>2478.3902439024387</v>
       </c>
       <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>2747.8715203426123</v>
+        <v>3017.1707317073169</v>
       </c>
       <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>2747.8715203426123</v>
+        <v>3017.1707317073169</v>
       </c>
       <c r="Q36" s="4">
         <f>Q35*B38</f>
-        <v>1955.2162740899357</v>
+        <v>1993.4878048780488</v>
       </c>
       <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>2853.5588865096361</v>
+        <v>3124.9268292682927</v>
       </c>
       <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>2272.2783725910062</v>
+        <v>2532.2682926829266</v>
       </c>
       <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>3117.7773019271949</v>
+        <v>3394.3170731707314</v>
       </c>
       <c r="U36" s="8"/>
     </row>
@@ -2999,43 +3043,43 @@
       <c r="J37" s="4"/>
       <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>1154.2526766595288</v>
+        <v>2517.3658536585367</v>
       </c>
       <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>689.56531049250543</v>
+        <v>646.12195121951208</v>
       </c>
       <c r="M37" s="20">
         <f>B9-M36</f>
-        <v>-662.43468950749457</v>
+        <v>-759.75609756097538</v>
       </c>
       <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>-712.80942184154173</v>
+        <v>-760.39024390243867</v>
       </c>
       <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>394.12847965738774</v>
+        <v>274.82926829268308</v>
       </c>
       <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>-247.87152034261226</v>
+        <v>-517.17073170731692</v>
       </c>
       <c r="Q37" s="17">
         <f>B8-Q36</f>
-        <v>544.78372591006428</v>
+        <v>506.51219512195121</v>
       </c>
       <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>-670.55888650963607</v>
+        <v>-941.92682926829275</v>
       </c>
       <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>242.72162740899375</v>
+        <v>-17.268292682926585</v>
       </c>
       <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>-617.77730192719491</v>
+        <v>-894.31707317073142</v>
       </c>
       <c r="U37" s="8"/>
     </row>
@@ -3045,7 +3089,7 @@
       </c>
       <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>52.843683083511777</v>
+        <v>53.878048780487802</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>

</xml_diff>

<commit_message>
updated for 30 tarikh
</commit_message>
<xml_diff>
--- a/October2021.xlsx
+++ b/October2021.xlsx
@@ -708,7 +708,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -788,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>4888</v>
+        <v>5688</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4">
@@ -1185,7 +1185,7 @@
         <v>2</v>
       </c>
       <c r="U8" s="8">
-        <f t="shared" ref="U8:U34" si="2">SUM(K8:T8)</f>
+        <f t="shared" ref="U8:U32" si="2">SUM(K8:T8)</f>
         <v>17</v>
       </c>
       <c r="X8" s="21">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="B13" s="10">
         <f>SUM(B3:B12)</f>
-        <v>26562</v>
+        <v>27362</v>
       </c>
       <c r="C13" s="26">
         <f>SUM(C3:C12)</f>
@@ -2756,7 +2756,9 @@
       <c r="E32" s="6">
         <v>44498</v>
       </c>
-      <c r="F32" s="7"/>
+      <c r="F32" s="7">
+        <v>500</v>
+      </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
@@ -2819,26 +2821,48 @@
       <c r="E33" s="6">
         <v>44499</v>
       </c>
-      <c r="F33" s="7"/>
+      <c r="F33" s="7">
+        <v>300</v>
+      </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="6">
         <v>44499</v>
       </c>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
+      <c r="K33" s="4">
+        <v>0</v>
+      </c>
+      <c r="L33" s="4">
+        <v>0</v>
+      </c>
+      <c r="M33" s="9">
+        <v>0</v>
+      </c>
+      <c r="N33" s="4">
+        <v>0</v>
+      </c>
+      <c r="O33" s="4">
+        <v>2</v>
+      </c>
+      <c r="P33" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>2</v>
+      </c>
+      <c r="R33" s="4">
+        <v>2</v>
+      </c>
+      <c r="S33" s="4">
+        <v>2</v>
+      </c>
+      <c r="T33" s="4">
+        <v>4</v>
+      </c>
       <c r="U33" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>SUM(K33:T33)</f>
+        <v>14</v>
       </c>
       <c r="X33" s="21">
         <v>44499</v>
@@ -2869,18 +2893,38 @@
       <c r="J34" s="6">
         <v>44500</v>
       </c>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
+      <c r="K34" s="4">
+        <v>0</v>
+      </c>
+      <c r="L34" s="4">
+        <v>0</v>
+      </c>
+      <c r="M34" s="9">
+        <v>0</v>
+      </c>
+      <c r="N34" s="4">
+        <v>0</v>
+      </c>
+      <c r="O34" s="4">
+        <v>0</v>
+      </c>
+      <c r="P34" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="4">
+        <v>0</v>
+      </c>
+      <c r="R34" s="4">
+        <v>0</v>
+      </c>
+      <c r="S34" s="4">
+        <v>0</v>
+      </c>
+      <c r="T34" s="4">
+        <v>0</v>
+      </c>
       <c r="U34" s="8">
-        <f t="shared" si="2"/>
+        <f>SUM(K34:T34)</f>
         <v>0</v>
       </c>
       <c r="X34" s="21">
@@ -2907,7 +2951,7 @@
       </c>
       <c r="F35" s="12">
         <f>SUM(F4:F34)</f>
-        <v>26508</v>
+        <v>27308</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -2916,15 +2960,15 @@
         <v>14</v>
       </c>
       <c r="K35" s="14">
-        <f>SUM(K4:K34)</f>
+        <f t="shared" ref="K35:U35" si="3">SUM(K4:K34)</f>
         <v>44</v>
       </c>
       <c r="L35" s="14">
-        <f>SUM(L4:L34)</f>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="M35" s="14">
-        <f t="shared" ref="M35:T35" si="3">SUM(M4:M34)</f>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="N35" s="14">
@@ -2933,31 +2977,31 @@
       </c>
       <c r="O35" s="14">
         <f t="shared" si="3"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="3"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q35" s="14">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="R35" s="14">
         <f t="shared" si="3"/>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S35" s="14">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="T35" s="14">
         <f t="shared" si="3"/>
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="U35" s="15">
-        <f>SUM(U4:U34)</f>
-        <v>492</v>
+        <f t="shared" si="3"/>
+        <v>506</v>
       </c>
       <c r="X35" s="24" t="s">
         <v>28</v>
@@ -2990,43 +3034,43 @@
       </c>
       <c r="K36" s="4">
         <f>K35*B38</f>
-        <v>2370.6341463414633</v>
+        <v>2374.608695652174</v>
       </c>
       <c r="L36" s="4">
         <f>L35*B38</f>
-        <v>2262.8780487804879</v>
+        <v>2266.671936758893</v>
       </c>
       <c r="M36" s="4">
         <f>M35*B38</f>
-        <v>2316.7560975609754</v>
+        <v>2320.6403162055335</v>
       </c>
       <c r="N36" s="4">
         <f>N35*B38</f>
-        <v>2478.3902439024387</v>
+        <v>2482.5454545454545</v>
       </c>
       <c r="O36" s="4">
         <f>O35*B38</f>
-        <v>3017.1707317073169</v>
+        <v>3130.166007905138</v>
       </c>
       <c r="P36" s="4">
         <f>P35*B38</f>
-        <v>3017.1707317073169</v>
+        <v>3130.166007905138</v>
       </c>
       <c r="Q36" s="4">
         <f>Q35*B38</f>
-        <v>1993.4878048780488</v>
+        <v>2104.766798418972</v>
       </c>
       <c r="R36" s="4">
         <f>R35*B38</f>
-        <v>3124.9268292682927</v>
+        <v>3238.102766798419</v>
       </c>
       <c r="S36" s="4">
         <f>S35*B38</f>
-        <v>2532.2682926829266</v>
+        <v>2644.4505928853755</v>
       </c>
       <c r="T36" s="4">
         <f>T35*B38</f>
-        <v>3394.3170731707314</v>
+        <v>3615.881422924901</v>
       </c>
       <c r="U36" s="8"/>
     </row>
@@ -3043,43 +3087,43 @@
       <c r="J37" s="4"/>
       <c r="K37" s="17">
         <f>B3-K36</f>
-        <v>2517.3658536585367</v>
+        <v>3313.391304347826</v>
       </c>
       <c r="L37" s="17">
         <f>B4-L36</f>
-        <v>646.12195121951208</v>
+        <v>642.32806324110697</v>
       </c>
       <c r="M37" s="20">
         <f>B9-M36</f>
-        <v>-759.75609756097538</v>
+        <v>-763.64031620553351</v>
       </c>
       <c r="N37" s="17">
         <f>B6-N36</f>
-        <v>-760.39024390243867</v>
+        <v>-764.5454545454545</v>
       </c>
       <c r="O37" s="17">
         <f>B5-O36</f>
-        <v>274.82926829268308</v>
+        <v>161.83399209486197</v>
       </c>
       <c r="P37" s="17">
         <f>B7-P36</f>
-        <v>-517.17073170731692</v>
+        <v>-630.16600790513803</v>
       </c>
       <c r="Q37" s="17">
         <f>B8-Q36</f>
-        <v>506.51219512195121</v>
+        <v>395.23320158102797</v>
       </c>
       <c r="R37" s="17">
         <f>B10-R36</f>
-        <v>-941.92682926829275</v>
+        <v>-1055.102766798419</v>
       </c>
       <c r="S37" s="17">
         <f>B11-S36</f>
-        <v>-17.268292682926585</v>
+        <v>-129.4505928853755</v>
       </c>
       <c r="T37" s="17">
         <f>B12-T36</f>
-        <v>-894.31707317073142</v>
+        <v>-1115.881422924901</v>
       </c>
       <c r="U37" s="8"/>
     </row>
@@ -3089,7 +3133,7 @@
       </c>
       <c r="B38" s="18">
         <f>F35/U35</f>
-        <v>53.878048780487802</v>
+        <v>53.968379446640313</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>

</xml_diff>